<commit_message>
Add report, update excel document
</commit_message>
<xml_diff>
--- a/runtimeTbl.xlsx
+++ b/runtimeTbl.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>number of integers N</t>
   </si>
@@ -43,10 +43,16 @@
     <t>heap sort</t>
   </si>
   <si>
+    <t>O(NlogN)</t>
+  </si>
+  <si>
     <t>merge sort</t>
   </si>
   <si>
     <t>quick sort (no cutoff)</t>
+  </si>
+  <si>
+    <t>O(N^2)</t>
   </si>
   <si>
     <t>insertion sort</t>
@@ -78,7 +84,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="30">
     <border/>
     <border>
       <left style="medium">
@@ -283,12 +289,9 @@
       </bottom>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -300,7 +303,21 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thick">
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
@@ -317,7 +334,7 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -331,7 +348,15 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -339,10 +364,13 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -350,28 +378,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -386,35 +392,7 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thick">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
@@ -428,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="38">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -484,20 +462,17 @@
     <xf borderId="19" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="20" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="21" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="22" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="23" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="20" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="21" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="21" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="22" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="24" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="23" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="25" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="24" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -506,22 +481,19 @@
     <xf borderId="10" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="26" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="25" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="27" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="26" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="27" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="28" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="29" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="30" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="28" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="29" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="31" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -666,3093 +638,3117 @@
       <c r="J4" s="24">
         <v>0.499638</v>
       </c>
-      <c r="K4" s="25"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="27"/>
+      <c r="K4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="25" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="25">
+        <v>0.003798</v>
+      </c>
+      <c r="C5" s="27">
+        <v>0.045693</v>
+      </c>
+      <c r="D5" s="28">
+        <v>0.531982</v>
+      </c>
+      <c r="E5" s="25">
+        <v>0.002967</v>
+      </c>
+      <c r="F5" s="27">
+        <v>0.037022</v>
+      </c>
+      <c r="G5" s="28">
+        <v>0.424316</v>
+      </c>
+      <c r="H5" s="25">
+        <v>0.002921</v>
+      </c>
+      <c r="I5" s="27">
+        <v>0.036574</v>
+      </c>
+      <c r="J5" s="28">
+        <v>0.42263</v>
+      </c>
+      <c r="K5" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="29">
-        <v>0.003798</v>
-      </c>
-      <c r="C5" s="30">
-        <v>0.045693</v>
-      </c>
-      <c r="D5" s="31">
-        <v>0.531982</v>
-      </c>
-      <c r="E5" s="29">
-        <v>0.002967</v>
-      </c>
-      <c r="F5" s="30">
-        <v>0.037022</v>
-      </c>
-      <c r="G5" s="31">
-        <v>0.424316</v>
-      </c>
-      <c r="H5" s="29">
-        <v>0.002921</v>
-      </c>
-      <c r="I5" s="30">
-        <v>0.036574</v>
-      </c>
-      <c r="J5" s="31">
-        <v>0.42263</v>
-      </c>
-      <c r="K5" s="25"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="27"/>
+      <c r="L5" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="25" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" ht="31.5" customHeight="1">
-      <c r="A6" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="33">
+      <c r="A6" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="30">
         <v>0.00204</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="31">
         <v>0.021112</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="32">
         <v>0.247706</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="30">
         <v>7.79E-4</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="31">
         <v>0.008281</v>
       </c>
-      <c r="G6" s="35">
+      <c r="G6" s="32">
         <v>0.106079</v>
       </c>
-      <c r="H6" s="33">
+      <c r="H6" s="30">
         <v>0.001251</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6" s="31">
         <v>0.016465</v>
       </c>
-      <c r="J6" s="35">
+      <c r="J6" s="32">
         <v>0.180965</v>
       </c>
-      <c r="K6" s="25"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="27"/>
+      <c r="K6" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="25" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="37">
+      <c r="A7" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="34">
         <v>0.286299</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="35">
         <v>28.5993</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="36">
         <v>2903.53</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="34">
         <v>1.95E-4</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="35">
         <v>0.001709</v>
       </c>
-      <c r="G7" s="39">
+      <c r="G7" s="36">
         <v>0.017284</v>
       </c>
-      <c r="H7" s="37">
+      <c r="H7" s="34">
         <v>0.600199</v>
       </c>
-      <c r="I7" s="38">
+      <c r="I7" s="35">
         <v>58.7056</v>
       </c>
-      <c r="J7" s="39">
+      <c r="J7" s="36">
         <v>5900.44</v>
       </c>
-      <c r="K7" s="40"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="42"/>
+      <c r="K7" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="34" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="43"/>
+      <c r="A8" s="37"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="43"/>
+      <c r="A9" s="37"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="43"/>
+      <c r="A10" s="37"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="43"/>
+      <c r="A11" s="37"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="43"/>
+      <c r="A12" s="37"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="43"/>
+      <c r="A13" s="37"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="43"/>
+      <c r="A14" s="37"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="43"/>
+      <c r="A15" s="37"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="43"/>
+      <c r="A16" s="37"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="43"/>
+      <c r="A17" s="37"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="43"/>
+      <c r="A18" s="37"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="43"/>
+      <c r="A19" s="37"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="43"/>
+      <c r="A20" s="37"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="43"/>
+      <c r="A21" s="37"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="43"/>
+      <c r="A22" s="37"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="43"/>
+      <c r="A23" s="37"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="43"/>
+      <c r="A24" s="37"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="43"/>
+      <c r="A25" s="37"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="43"/>
+      <c r="A26" s="37"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="43"/>
+      <c r="A27" s="37"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="43"/>
+      <c r="A28" s="37"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="43"/>
+      <c r="A29" s="37"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="43"/>
+      <c r="A30" s="37"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="43"/>
+      <c r="A31" s="37"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="43"/>
+      <c r="A32" s="37"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="43"/>
+      <c r="A33" s="37"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="43"/>
+      <c r="A34" s="37"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="43"/>
+      <c r="A35" s="37"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="43"/>
+      <c r="A36" s="37"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="43"/>
+      <c r="A37" s="37"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="43"/>
+      <c r="A38" s="37"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="43"/>
+      <c r="A39" s="37"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="43"/>
+      <c r="A40" s="37"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="43"/>
+      <c r="A41" s="37"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="43"/>
+      <c r="A42" s="37"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="43"/>
+      <c r="A43" s="37"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="43"/>
+      <c r="A44" s="37"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="43"/>
+      <c r="A45" s="37"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="43"/>
+      <c r="A46" s="37"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="43"/>
+      <c r="A47" s="37"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="43"/>
+      <c r="A48" s="37"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="43"/>
+      <c r="A49" s="37"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="43"/>
+      <c r="A50" s="37"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="43"/>
+      <c r="A51" s="37"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="43"/>
+      <c r="A52" s="37"/>
     </row>
     <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="43"/>
+      <c r="A53" s="37"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="43"/>
+      <c r="A54" s="37"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="43"/>
+      <c r="A55" s="37"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="43"/>
+      <c r="A56" s="37"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="43"/>
+      <c r="A57" s="37"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="43"/>
+      <c r="A58" s="37"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="43"/>
+      <c r="A59" s="37"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="43"/>
+      <c r="A60" s="37"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="43"/>
+      <c r="A61" s="37"/>
     </row>
     <row r="62" ht="14.25" customHeight="1">
-      <c r="A62" s="43"/>
+      <c r="A62" s="37"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" s="43"/>
+      <c r="A63" s="37"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" s="43"/>
+      <c r="A64" s="37"/>
     </row>
     <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="43"/>
+      <c r="A65" s="37"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="43"/>
+      <c r="A66" s="37"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="43"/>
+      <c r="A67" s="37"/>
     </row>
     <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="43"/>
+      <c r="A68" s="37"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" s="43"/>
+      <c r="A69" s="37"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
-      <c r="A70" s="43"/>
+      <c r="A70" s="37"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="43"/>
+      <c r="A71" s="37"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="43"/>
+      <c r="A72" s="37"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="43"/>
+      <c r="A73" s="37"/>
     </row>
     <row r="74" ht="14.25" customHeight="1">
-      <c r="A74" s="43"/>
+      <c r="A74" s="37"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="43"/>
+      <c r="A75" s="37"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="43"/>
+      <c r="A76" s="37"/>
     </row>
     <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="43"/>
+      <c r="A77" s="37"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="43"/>
+      <c r="A78" s="37"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" s="43"/>
+      <c r="A79" s="37"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" s="43"/>
+      <c r="A80" s="37"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
-      <c r="A81" s="43"/>
+      <c r="A81" s="37"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
-      <c r="A82" s="43"/>
+      <c r="A82" s="37"/>
     </row>
     <row r="83" ht="14.25" customHeight="1">
-      <c r="A83" s="43"/>
+      <c r="A83" s="37"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
-      <c r="A84" s="43"/>
+      <c r="A84" s="37"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
-      <c r="A85" s="43"/>
+      <c r="A85" s="37"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="43"/>
+      <c r="A86" s="37"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
-      <c r="A87" s="43"/>
+      <c r="A87" s="37"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="43"/>
+      <c r="A88" s="37"/>
     </row>
     <row r="89" ht="14.25" customHeight="1">
-      <c r="A89" s="43"/>
+      <c r="A89" s="37"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" s="43"/>
+      <c r="A90" s="37"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" s="43"/>
+      <c r="A91" s="37"/>
     </row>
     <row r="92" ht="14.25" customHeight="1">
-      <c r="A92" s="43"/>
+      <c r="A92" s="37"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
-      <c r="A93" s="43"/>
+      <c r="A93" s="37"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
-      <c r="A94" s="43"/>
+      <c r="A94" s="37"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="43"/>
+      <c r="A95" s="37"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" s="43"/>
+      <c r="A96" s="37"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" s="43"/>
+      <c r="A97" s="37"/>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" s="43"/>
+      <c r="A98" s="37"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
-      <c r="A99" s="43"/>
+      <c r="A99" s="37"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
-      <c r="A100" s="43"/>
+      <c r="A100" s="37"/>
     </row>
     <row r="101" ht="14.25" customHeight="1">
-      <c r="A101" s="43"/>
+      <c r="A101" s="37"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
-      <c r="A102" s="43"/>
+      <c r="A102" s="37"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
-      <c r="A103" s="43"/>
+      <c r="A103" s="37"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" s="43"/>
+      <c r="A104" s="37"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
-      <c r="A105" s="43"/>
+      <c r="A105" s="37"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
-      <c r="A106" s="43"/>
+      <c r="A106" s="37"/>
     </row>
     <row r="107" ht="14.25" customHeight="1">
-      <c r="A107" s="43"/>
+      <c r="A107" s="37"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
-      <c r="A108" s="43"/>
+      <c r="A108" s="37"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
-      <c r="A109" s="43"/>
+      <c r="A109" s="37"/>
     </row>
     <row r="110" ht="14.25" customHeight="1">
-      <c r="A110" s="43"/>
+      <c r="A110" s="37"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
-      <c r="A111" s="43"/>
+      <c r="A111" s="37"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
-      <c r="A112" s="43"/>
+      <c r="A112" s="37"/>
     </row>
     <row r="113" ht="14.25" customHeight="1">
-      <c r="A113" s="43"/>
+      <c r="A113" s="37"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
-      <c r="A114" s="43"/>
+      <c r="A114" s="37"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
-      <c r="A115" s="43"/>
+      <c r="A115" s="37"/>
     </row>
     <row r="116" ht="14.25" customHeight="1">
-      <c r="A116" s="43"/>
+      <c r="A116" s="37"/>
     </row>
     <row r="117" ht="14.25" customHeight="1">
-      <c r="A117" s="43"/>
+      <c r="A117" s="37"/>
     </row>
     <row r="118" ht="14.25" customHeight="1">
-      <c r="A118" s="43"/>
+      <c r="A118" s="37"/>
     </row>
     <row r="119" ht="14.25" customHeight="1">
-      <c r="A119" s="43"/>
+      <c r="A119" s="37"/>
     </row>
     <row r="120" ht="14.25" customHeight="1">
-      <c r="A120" s="43"/>
+      <c r="A120" s="37"/>
     </row>
     <row r="121" ht="14.25" customHeight="1">
-      <c r="A121" s="43"/>
+      <c r="A121" s="37"/>
     </row>
     <row r="122" ht="14.25" customHeight="1">
-      <c r="A122" s="43"/>
+      <c r="A122" s="37"/>
     </row>
     <row r="123" ht="14.25" customHeight="1">
-      <c r="A123" s="43"/>
+      <c r="A123" s="37"/>
     </row>
     <row r="124" ht="14.25" customHeight="1">
-      <c r="A124" s="43"/>
+      <c r="A124" s="37"/>
     </row>
     <row r="125" ht="14.25" customHeight="1">
-      <c r="A125" s="43"/>
+      <c r="A125" s="37"/>
     </row>
     <row r="126" ht="14.25" customHeight="1">
-      <c r="A126" s="43"/>
+      <c r="A126" s="37"/>
     </row>
     <row r="127" ht="14.25" customHeight="1">
-      <c r="A127" s="43"/>
+      <c r="A127" s="37"/>
     </row>
     <row r="128" ht="14.25" customHeight="1">
-      <c r="A128" s="43"/>
+      <c r="A128" s="37"/>
     </row>
     <row r="129" ht="14.25" customHeight="1">
-      <c r="A129" s="43"/>
+      <c r="A129" s="37"/>
     </row>
     <row r="130" ht="14.25" customHeight="1">
-      <c r="A130" s="43"/>
+      <c r="A130" s="37"/>
     </row>
     <row r="131" ht="14.25" customHeight="1">
-      <c r="A131" s="43"/>
+      <c r="A131" s="37"/>
     </row>
     <row r="132" ht="14.25" customHeight="1">
-      <c r="A132" s="43"/>
+      <c r="A132" s="37"/>
     </row>
     <row r="133" ht="14.25" customHeight="1">
-      <c r="A133" s="43"/>
+      <c r="A133" s="37"/>
     </row>
     <row r="134" ht="14.25" customHeight="1">
-      <c r="A134" s="43"/>
+      <c r="A134" s="37"/>
     </row>
     <row r="135" ht="14.25" customHeight="1">
-      <c r="A135" s="43"/>
+      <c r="A135" s="37"/>
     </row>
     <row r="136" ht="14.25" customHeight="1">
-      <c r="A136" s="43"/>
+      <c r="A136" s="37"/>
     </row>
     <row r="137" ht="14.25" customHeight="1">
-      <c r="A137" s="43"/>
+      <c r="A137" s="37"/>
     </row>
     <row r="138" ht="14.25" customHeight="1">
-      <c r="A138" s="43"/>
+      <c r="A138" s="37"/>
     </row>
     <row r="139" ht="14.25" customHeight="1">
-      <c r="A139" s="43"/>
+      <c r="A139" s="37"/>
     </row>
     <row r="140" ht="14.25" customHeight="1">
-      <c r="A140" s="43"/>
+      <c r="A140" s="37"/>
     </row>
     <row r="141" ht="14.25" customHeight="1">
-      <c r="A141" s="43"/>
+      <c r="A141" s="37"/>
     </row>
     <row r="142" ht="14.25" customHeight="1">
-      <c r="A142" s="43"/>
+      <c r="A142" s="37"/>
     </row>
     <row r="143" ht="14.25" customHeight="1">
-      <c r="A143" s="43"/>
+      <c r="A143" s="37"/>
     </row>
     <row r="144" ht="14.25" customHeight="1">
-      <c r="A144" s="43"/>
+      <c r="A144" s="37"/>
     </row>
     <row r="145" ht="14.25" customHeight="1">
-      <c r="A145" s="43"/>
+      <c r="A145" s="37"/>
     </row>
     <row r="146" ht="14.25" customHeight="1">
-      <c r="A146" s="43"/>
+      <c r="A146" s="37"/>
     </row>
     <row r="147" ht="14.25" customHeight="1">
-      <c r="A147" s="43"/>
+      <c r="A147" s="37"/>
     </row>
     <row r="148" ht="14.25" customHeight="1">
-      <c r="A148" s="43"/>
+      <c r="A148" s="37"/>
     </row>
     <row r="149" ht="14.25" customHeight="1">
-      <c r="A149" s="43"/>
+      <c r="A149" s="37"/>
     </row>
     <row r="150" ht="14.25" customHeight="1">
-      <c r="A150" s="43"/>
+      <c r="A150" s="37"/>
     </row>
     <row r="151" ht="14.25" customHeight="1">
-      <c r="A151" s="43"/>
+      <c r="A151" s="37"/>
     </row>
     <row r="152" ht="14.25" customHeight="1">
-      <c r="A152" s="43"/>
+      <c r="A152" s="37"/>
     </row>
     <row r="153" ht="14.25" customHeight="1">
-      <c r="A153" s="43"/>
+      <c r="A153" s="37"/>
     </row>
     <row r="154" ht="14.25" customHeight="1">
-      <c r="A154" s="43"/>
+      <c r="A154" s="37"/>
     </row>
     <row r="155" ht="14.25" customHeight="1">
-      <c r="A155" s="43"/>
+      <c r="A155" s="37"/>
     </row>
     <row r="156" ht="14.25" customHeight="1">
-      <c r="A156" s="43"/>
+      <c r="A156" s="37"/>
     </row>
     <row r="157" ht="14.25" customHeight="1">
-      <c r="A157" s="43"/>
+      <c r="A157" s="37"/>
     </row>
     <row r="158" ht="14.25" customHeight="1">
-      <c r="A158" s="43"/>
+      <c r="A158" s="37"/>
     </row>
     <row r="159" ht="14.25" customHeight="1">
-      <c r="A159" s="43"/>
+      <c r="A159" s="37"/>
     </row>
     <row r="160" ht="14.25" customHeight="1">
-      <c r="A160" s="43"/>
+      <c r="A160" s="37"/>
     </row>
     <row r="161" ht="14.25" customHeight="1">
-      <c r="A161" s="43"/>
+      <c r="A161" s="37"/>
     </row>
     <row r="162" ht="14.25" customHeight="1">
-      <c r="A162" s="43"/>
+      <c r="A162" s="37"/>
     </row>
     <row r="163" ht="14.25" customHeight="1">
-      <c r="A163" s="43"/>
+      <c r="A163" s="37"/>
     </row>
     <row r="164" ht="14.25" customHeight="1">
-      <c r="A164" s="43"/>
+      <c r="A164" s="37"/>
     </row>
     <row r="165" ht="14.25" customHeight="1">
-      <c r="A165" s="43"/>
+      <c r="A165" s="37"/>
     </row>
     <row r="166" ht="14.25" customHeight="1">
-      <c r="A166" s="43"/>
+      <c r="A166" s="37"/>
     </row>
     <row r="167" ht="14.25" customHeight="1">
-      <c r="A167" s="43"/>
+      <c r="A167" s="37"/>
     </row>
     <row r="168" ht="14.25" customHeight="1">
-      <c r="A168" s="43"/>
+      <c r="A168" s="37"/>
     </row>
     <row r="169" ht="14.25" customHeight="1">
-      <c r="A169" s="43"/>
+      <c r="A169" s="37"/>
     </row>
     <row r="170" ht="14.25" customHeight="1">
-      <c r="A170" s="43"/>
+      <c r="A170" s="37"/>
     </row>
     <row r="171" ht="14.25" customHeight="1">
-      <c r="A171" s="43"/>
+      <c r="A171" s="37"/>
     </row>
     <row r="172" ht="14.25" customHeight="1">
-      <c r="A172" s="43"/>
+      <c r="A172" s="37"/>
     </row>
     <row r="173" ht="14.25" customHeight="1">
-      <c r="A173" s="43"/>
+      <c r="A173" s="37"/>
     </row>
     <row r="174" ht="14.25" customHeight="1">
-      <c r="A174" s="43"/>
+      <c r="A174" s="37"/>
     </row>
     <row r="175" ht="14.25" customHeight="1">
-      <c r="A175" s="43"/>
+      <c r="A175" s="37"/>
     </row>
     <row r="176" ht="14.25" customHeight="1">
-      <c r="A176" s="43"/>
+      <c r="A176" s="37"/>
     </row>
     <row r="177" ht="14.25" customHeight="1">
-      <c r="A177" s="43"/>
+      <c r="A177" s="37"/>
     </row>
     <row r="178" ht="14.25" customHeight="1">
-      <c r="A178" s="43"/>
+      <c r="A178" s="37"/>
     </row>
     <row r="179" ht="14.25" customHeight="1">
-      <c r="A179" s="43"/>
+      <c r="A179" s="37"/>
     </row>
     <row r="180" ht="14.25" customHeight="1">
-      <c r="A180" s="43"/>
+      <c r="A180" s="37"/>
     </row>
     <row r="181" ht="14.25" customHeight="1">
-      <c r="A181" s="43"/>
+      <c r="A181" s="37"/>
     </row>
     <row r="182" ht="14.25" customHeight="1">
-      <c r="A182" s="43"/>
+      <c r="A182" s="37"/>
     </row>
     <row r="183" ht="14.25" customHeight="1">
-      <c r="A183" s="43"/>
+      <c r="A183" s="37"/>
     </row>
     <row r="184" ht="14.25" customHeight="1">
-      <c r="A184" s="43"/>
+      <c r="A184" s="37"/>
     </row>
     <row r="185" ht="14.25" customHeight="1">
-      <c r="A185" s="43"/>
+      <c r="A185" s="37"/>
     </row>
     <row r="186" ht="14.25" customHeight="1">
-      <c r="A186" s="43"/>
+      <c r="A186" s="37"/>
     </row>
     <row r="187" ht="14.25" customHeight="1">
-      <c r="A187" s="43"/>
+      <c r="A187" s="37"/>
     </row>
     <row r="188" ht="14.25" customHeight="1">
-      <c r="A188" s="43"/>
+      <c r="A188" s="37"/>
     </row>
     <row r="189" ht="14.25" customHeight="1">
-      <c r="A189" s="43"/>
+      <c r="A189" s="37"/>
     </row>
     <row r="190" ht="14.25" customHeight="1">
-      <c r="A190" s="43"/>
+      <c r="A190" s="37"/>
     </row>
     <row r="191" ht="14.25" customHeight="1">
-      <c r="A191" s="43"/>
+      <c r="A191" s="37"/>
     </row>
     <row r="192" ht="14.25" customHeight="1">
-      <c r="A192" s="43"/>
+      <c r="A192" s="37"/>
     </row>
     <row r="193" ht="14.25" customHeight="1">
-      <c r="A193" s="43"/>
+      <c r="A193" s="37"/>
     </row>
     <row r="194" ht="14.25" customHeight="1">
-      <c r="A194" s="43"/>
+      <c r="A194" s="37"/>
     </row>
     <row r="195" ht="14.25" customHeight="1">
-      <c r="A195" s="43"/>
+      <c r="A195" s="37"/>
     </row>
     <row r="196" ht="14.25" customHeight="1">
-      <c r="A196" s="43"/>
+      <c r="A196" s="37"/>
     </row>
     <row r="197" ht="14.25" customHeight="1">
-      <c r="A197" s="43"/>
+      <c r="A197" s="37"/>
     </row>
     <row r="198" ht="14.25" customHeight="1">
-      <c r="A198" s="43"/>
+      <c r="A198" s="37"/>
     </row>
     <row r="199" ht="14.25" customHeight="1">
-      <c r="A199" s="43"/>
+      <c r="A199" s="37"/>
     </row>
     <row r="200" ht="14.25" customHeight="1">
-      <c r="A200" s="43"/>
+      <c r="A200" s="37"/>
     </row>
     <row r="201" ht="14.25" customHeight="1">
-      <c r="A201" s="43"/>
+      <c r="A201" s="37"/>
     </row>
     <row r="202" ht="14.25" customHeight="1">
-      <c r="A202" s="43"/>
+      <c r="A202" s="37"/>
     </row>
     <row r="203" ht="14.25" customHeight="1">
-      <c r="A203" s="43"/>
+      <c r="A203" s="37"/>
     </row>
     <row r="204" ht="14.25" customHeight="1">
-      <c r="A204" s="43"/>
+      <c r="A204" s="37"/>
     </row>
     <row r="205" ht="14.25" customHeight="1">
-      <c r="A205" s="43"/>
+      <c r="A205" s="37"/>
     </row>
     <row r="206" ht="14.25" customHeight="1">
-      <c r="A206" s="43"/>
+      <c r="A206" s="37"/>
     </row>
     <row r="207" ht="14.25" customHeight="1">
-      <c r="A207" s="43"/>
+      <c r="A207" s="37"/>
     </row>
     <row r="208" ht="14.25" customHeight="1">
-      <c r="A208" s="43"/>
+      <c r="A208" s="37"/>
     </row>
     <row r="209" ht="14.25" customHeight="1">
-      <c r="A209" s="43"/>
+      <c r="A209" s="37"/>
     </row>
     <row r="210" ht="14.25" customHeight="1">
-      <c r="A210" s="43"/>
+      <c r="A210" s="37"/>
     </row>
     <row r="211" ht="14.25" customHeight="1">
-      <c r="A211" s="43"/>
+      <c r="A211" s="37"/>
     </row>
     <row r="212" ht="14.25" customHeight="1">
-      <c r="A212" s="43"/>
+      <c r="A212" s="37"/>
     </row>
     <row r="213" ht="14.25" customHeight="1">
-      <c r="A213" s="43"/>
+      <c r="A213" s="37"/>
     </row>
     <row r="214" ht="14.25" customHeight="1">
-      <c r="A214" s="43"/>
+      <c r="A214" s="37"/>
     </row>
     <row r="215" ht="14.25" customHeight="1">
-      <c r="A215" s="43"/>
+      <c r="A215" s="37"/>
     </row>
     <row r="216" ht="14.25" customHeight="1">
-      <c r="A216" s="43"/>
+      <c r="A216" s="37"/>
     </row>
     <row r="217" ht="14.25" customHeight="1">
-      <c r="A217" s="43"/>
+      <c r="A217" s="37"/>
     </row>
     <row r="218" ht="14.25" customHeight="1">
-      <c r="A218" s="43"/>
+      <c r="A218" s="37"/>
     </row>
     <row r="219" ht="14.25" customHeight="1">
-      <c r="A219" s="43"/>
+      <c r="A219" s="37"/>
     </row>
     <row r="220" ht="14.25" customHeight="1">
-      <c r="A220" s="43"/>
+      <c r="A220" s="37"/>
     </row>
     <row r="221" ht="14.25" customHeight="1">
-      <c r="A221" s="43"/>
+      <c r="A221" s="37"/>
     </row>
     <row r="222" ht="14.25" customHeight="1">
-      <c r="A222" s="43"/>
+      <c r="A222" s="37"/>
     </row>
     <row r="223" ht="14.25" customHeight="1">
-      <c r="A223" s="43"/>
+      <c r="A223" s="37"/>
     </row>
     <row r="224" ht="14.25" customHeight="1">
-      <c r="A224" s="43"/>
+      <c r="A224" s="37"/>
     </row>
     <row r="225" ht="14.25" customHeight="1">
-      <c r="A225" s="43"/>
+      <c r="A225" s="37"/>
     </row>
     <row r="226" ht="14.25" customHeight="1">
-      <c r="A226" s="43"/>
+      <c r="A226" s="37"/>
     </row>
     <row r="227" ht="14.25" customHeight="1">
-      <c r="A227" s="43"/>
+      <c r="A227" s="37"/>
     </row>
     <row r="228" ht="14.25" customHeight="1">
-      <c r="A228" s="43"/>
+      <c r="A228" s="37"/>
     </row>
     <row r="229" ht="14.25" customHeight="1">
-      <c r="A229" s="43"/>
+      <c r="A229" s="37"/>
     </row>
     <row r="230" ht="14.25" customHeight="1">
-      <c r="A230" s="43"/>
+      <c r="A230" s="37"/>
     </row>
     <row r="231" ht="14.25" customHeight="1">
-      <c r="A231" s="43"/>
+      <c r="A231" s="37"/>
     </row>
     <row r="232" ht="14.25" customHeight="1">
-      <c r="A232" s="43"/>
+      <c r="A232" s="37"/>
     </row>
     <row r="233" ht="14.25" customHeight="1">
-      <c r="A233" s="43"/>
+      <c r="A233" s="37"/>
     </row>
     <row r="234" ht="14.25" customHeight="1">
-      <c r="A234" s="43"/>
+      <c r="A234" s="37"/>
     </row>
     <row r="235" ht="14.25" customHeight="1">
-      <c r="A235" s="43"/>
+      <c r="A235" s="37"/>
     </row>
     <row r="236" ht="14.25" customHeight="1">
-      <c r="A236" s="43"/>
+      <c r="A236" s="37"/>
     </row>
     <row r="237" ht="14.25" customHeight="1">
-      <c r="A237" s="43"/>
+      <c r="A237" s="37"/>
     </row>
     <row r="238" ht="14.25" customHeight="1">
-      <c r="A238" s="43"/>
+      <c r="A238" s="37"/>
     </row>
     <row r="239" ht="14.25" customHeight="1">
-      <c r="A239" s="43"/>
+      <c r="A239" s="37"/>
     </row>
     <row r="240" ht="14.25" customHeight="1">
-      <c r="A240" s="43"/>
+      <c r="A240" s="37"/>
     </row>
     <row r="241" ht="14.25" customHeight="1">
-      <c r="A241" s="43"/>
+      <c r="A241" s="37"/>
     </row>
     <row r="242" ht="14.25" customHeight="1">
-      <c r="A242" s="43"/>
+      <c r="A242" s="37"/>
     </row>
     <row r="243" ht="14.25" customHeight="1">
-      <c r="A243" s="43"/>
+      <c r="A243" s="37"/>
     </row>
     <row r="244" ht="14.25" customHeight="1">
-      <c r="A244" s="43"/>
+      <c r="A244" s="37"/>
     </row>
     <row r="245" ht="14.25" customHeight="1">
-      <c r="A245" s="43"/>
+      <c r="A245" s="37"/>
     </row>
     <row r="246" ht="14.25" customHeight="1">
-      <c r="A246" s="43"/>
+      <c r="A246" s="37"/>
     </row>
     <row r="247" ht="14.25" customHeight="1">
-      <c r="A247" s="43"/>
+      <c r="A247" s="37"/>
     </row>
     <row r="248" ht="14.25" customHeight="1">
-      <c r="A248" s="43"/>
+      <c r="A248" s="37"/>
     </row>
     <row r="249" ht="14.25" customHeight="1">
-      <c r="A249" s="43"/>
+      <c r="A249" s="37"/>
     </row>
     <row r="250" ht="14.25" customHeight="1">
-      <c r="A250" s="43"/>
+      <c r="A250" s="37"/>
     </row>
     <row r="251" ht="14.25" customHeight="1">
-      <c r="A251" s="43"/>
+      <c r="A251" s="37"/>
     </row>
     <row r="252" ht="14.25" customHeight="1">
-      <c r="A252" s="43"/>
+      <c r="A252" s="37"/>
     </row>
     <row r="253" ht="14.25" customHeight="1">
-      <c r="A253" s="43"/>
+      <c r="A253" s="37"/>
     </row>
     <row r="254" ht="14.25" customHeight="1">
-      <c r="A254" s="43"/>
+      <c r="A254" s="37"/>
     </row>
     <row r="255" ht="14.25" customHeight="1">
-      <c r="A255" s="43"/>
+      <c r="A255" s="37"/>
     </row>
     <row r="256" ht="14.25" customHeight="1">
-      <c r="A256" s="43"/>
+      <c r="A256" s="37"/>
     </row>
     <row r="257" ht="14.25" customHeight="1">
-      <c r="A257" s="43"/>
+      <c r="A257" s="37"/>
     </row>
     <row r="258" ht="14.25" customHeight="1">
-      <c r="A258" s="43"/>
+      <c r="A258" s="37"/>
     </row>
     <row r="259" ht="14.25" customHeight="1">
-      <c r="A259" s="43"/>
+      <c r="A259" s="37"/>
     </row>
     <row r="260" ht="14.25" customHeight="1">
-      <c r="A260" s="43"/>
+      <c r="A260" s="37"/>
     </row>
     <row r="261" ht="14.25" customHeight="1">
-      <c r="A261" s="43"/>
+      <c r="A261" s="37"/>
     </row>
     <row r="262" ht="14.25" customHeight="1">
-      <c r="A262" s="43"/>
+      <c r="A262" s="37"/>
     </row>
     <row r="263" ht="14.25" customHeight="1">
-      <c r="A263" s="43"/>
+      <c r="A263" s="37"/>
     </row>
     <row r="264" ht="14.25" customHeight="1">
-      <c r="A264" s="43"/>
+      <c r="A264" s="37"/>
     </row>
     <row r="265" ht="14.25" customHeight="1">
-      <c r="A265" s="43"/>
+      <c r="A265" s="37"/>
     </row>
     <row r="266" ht="14.25" customHeight="1">
-      <c r="A266" s="43"/>
+      <c r="A266" s="37"/>
     </row>
     <row r="267" ht="14.25" customHeight="1">
-      <c r="A267" s="43"/>
+      <c r="A267" s="37"/>
     </row>
     <row r="268" ht="14.25" customHeight="1">
-      <c r="A268" s="43"/>
+      <c r="A268" s="37"/>
     </row>
     <row r="269" ht="14.25" customHeight="1">
-      <c r="A269" s="43"/>
+      <c r="A269" s="37"/>
     </row>
     <row r="270" ht="14.25" customHeight="1">
-      <c r="A270" s="43"/>
+      <c r="A270" s="37"/>
     </row>
     <row r="271" ht="14.25" customHeight="1">
-      <c r="A271" s="43"/>
+      <c r="A271" s="37"/>
     </row>
     <row r="272" ht="14.25" customHeight="1">
-      <c r="A272" s="43"/>
+      <c r="A272" s="37"/>
     </row>
     <row r="273" ht="14.25" customHeight="1">
-      <c r="A273" s="43"/>
+      <c r="A273" s="37"/>
     </row>
     <row r="274" ht="14.25" customHeight="1">
-      <c r="A274" s="43"/>
+      <c r="A274" s="37"/>
     </row>
     <row r="275" ht="14.25" customHeight="1">
-      <c r="A275" s="43"/>
+      <c r="A275" s="37"/>
     </row>
     <row r="276" ht="14.25" customHeight="1">
-      <c r="A276" s="43"/>
+      <c r="A276" s="37"/>
     </row>
     <row r="277" ht="14.25" customHeight="1">
-      <c r="A277" s="43"/>
+      <c r="A277" s="37"/>
     </row>
     <row r="278" ht="14.25" customHeight="1">
-      <c r="A278" s="43"/>
+      <c r="A278" s="37"/>
     </row>
     <row r="279" ht="14.25" customHeight="1">
-      <c r="A279" s="43"/>
+      <c r="A279" s="37"/>
     </row>
     <row r="280" ht="14.25" customHeight="1">
-      <c r="A280" s="43"/>
+      <c r="A280" s="37"/>
     </row>
     <row r="281" ht="14.25" customHeight="1">
-      <c r="A281" s="43"/>
+      <c r="A281" s="37"/>
     </row>
     <row r="282" ht="14.25" customHeight="1">
-      <c r="A282" s="43"/>
+      <c r="A282" s="37"/>
     </row>
     <row r="283" ht="14.25" customHeight="1">
-      <c r="A283" s="43"/>
+      <c r="A283" s="37"/>
     </row>
     <row r="284" ht="14.25" customHeight="1">
-      <c r="A284" s="43"/>
+      <c r="A284" s="37"/>
     </row>
     <row r="285" ht="14.25" customHeight="1">
-      <c r="A285" s="43"/>
+      <c r="A285" s="37"/>
     </row>
     <row r="286" ht="14.25" customHeight="1">
-      <c r="A286" s="43"/>
+      <c r="A286" s="37"/>
     </row>
     <row r="287" ht="14.25" customHeight="1">
-      <c r="A287" s="43"/>
+      <c r="A287" s="37"/>
     </row>
     <row r="288" ht="14.25" customHeight="1">
-      <c r="A288" s="43"/>
+      <c r="A288" s="37"/>
     </row>
     <row r="289" ht="14.25" customHeight="1">
-      <c r="A289" s="43"/>
+      <c r="A289" s="37"/>
     </row>
     <row r="290" ht="14.25" customHeight="1">
-      <c r="A290" s="43"/>
+      <c r="A290" s="37"/>
     </row>
     <row r="291" ht="14.25" customHeight="1">
-      <c r="A291" s="43"/>
+      <c r="A291" s="37"/>
     </row>
     <row r="292" ht="14.25" customHeight="1">
-      <c r="A292" s="43"/>
+      <c r="A292" s="37"/>
     </row>
     <row r="293" ht="14.25" customHeight="1">
-      <c r="A293" s="43"/>
+      <c r="A293" s="37"/>
     </row>
     <row r="294" ht="14.25" customHeight="1">
-      <c r="A294" s="43"/>
+      <c r="A294" s="37"/>
     </row>
     <row r="295" ht="14.25" customHeight="1">
-      <c r="A295" s="43"/>
+      <c r="A295" s="37"/>
     </row>
     <row r="296" ht="14.25" customHeight="1">
-      <c r="A296" s="43"/>
+      <c r="A296" s="37"/>
     </row>
     <row r="297" ht="14.25" customHeight="1">
-      <c r="A297" s="43"/>
+      <c r="A297" s="37"/>
     </row>
     <row r="298" ht="14.25" customHeight="1">
-      <c r="A298" s="43"/>
+      <c r="A298" s="37"/>
     </row>
     <row r="299" ht="14.25" customHeight="1">
-      <c r="A299" s="43"/>
+      <c r="A299" s="37"/>
     </row>
     <row r="300" ht="14.25" customHeight="1">
-      <c r="A300" s="43"/>
+      <c r="A300" s="37"/>
     </row>
     <row r="301" ht="14.25" customHeight="1">
-      <c r="A301" s="43"/>
+      <c r="A301" s="37"/>
     </row>
     <row r="302" ht="14.25" customHeight="1">
-      <c r="A302" s="43"/>
+      <c r="A302" s="37"/>
     </row>
     <row r="303" ht="14.25" customHeight="1">
-      <c r="A303" s="43"/>
+      <c r="A303" s="37"/>
     </row>
     <row r="304" ht="14.25" customHeight="1">
-      <c r="A304" s="43"/>
+      <c r="A304" s="37"/>
     </row>
     <row r="305" ht="14.25" customHeight="1">
-      <c r="A305" s="43"/>
+      <c r="A305" s="37"/>
     </row>
     <row r="306" ht="14.25" customHeight="1">
-      <c r="A306" s="43"/>
+      <c r="A306" s="37"/>
     </row>
     <row r="307" ht="14.25" customHeight="1">
-      <c r="A307" s="43"/>
+      <c r="A307" s="37"/>
     </row>
     <row r="308" ht="14.25" customHeight="1">
-      <c r="A308" s="43"/>
+      <c r="A308" s="37"/>
     </row>
     <row r="309" ht="14.25" customHeight="1">
-      <c r="A309" s="43"/>
+      <c r="A309" s="37"/>
     </row>
     <row r="310" ht="14.25" customHeight="1">
-      <c r="A310" s="43"/>
+      <c r="A310" s="37"/>
     </row>
     <row r="311" ht="14.25" customHeight="1">
-      <c r="A311" s="43"/>
+      <c r="A311" s="37"/>
     </row>
     <row r="312" ht="14.25" customHeight="1">
-      <c r="A312" s="43"/>
+      <c r="A312" s="37"/>
     </row>
     <row r="313" ht="14.25" customHeight="1">
-      <c r="A313" s="43"/>
+      <c r="A313" s="37"/>
     </row>
     <row r="314" ht="14.25" customHeight="1">
-      <c r="A314" s="43"/>
+      <c r="A314" s="37"/>
     </row>
     <row r="315" ht="14.25" customHeight="1">
-      <c r="A315" s="43"/>
+      <c r="A315" s="37"/>
     </row>
     <row r="316" ht="14.25" customHeight="1">
-      <c r="A316" s="43"/>
+      <c r="A316" s="37"/>
     </row>
     <row r="317" ht="14.25" customHeight="1">
-      <c r="A317" s="43"/>
+      <c r="A317" s="37"/>
     </row>
     <row r="318" ht="14.25" customHeight="1">
-      <c r="A318" s="43"/>
+      <c r="A318" s="37"/>
     </row>
     <row r="319" ht="14.25" customHeight="1">
-      <c r="A319" s="43"/>
+      <c r="A319" s="37"/>
     </row>
     <row r="320" ht="14.25" customHeight="1">
-      <c r="A320" s="43"/>
+      <c r="A320" s="37"/>
     </row>
     <row r="321" ht="14.25" customHeight="1">
-      <c r="A321" s="43"/>
+      <c r="A321" s="37"/>
     </row>
     <row r="322" ht="14.25" customHeight="1">
-      <c r="A322" s="43"/>
+      <c r="A322" s="37"/>
     </row>
     <row r="323" ht="14.25" customHeight="1">
-      <c r="A323" s="43"/>
+      <c r="A323" s="37"/>
     </row>
     <row r="324" ht="14.25" customHeight="1">
-      <c r="A324" s="43"/>
+      <c r="A324" s="37"/>
     </row>
     <row r="325" ht="14.25" customHeight="1">
-      <c r="A325" s="43"/>
+      <c r="A325" s="37"/>
     </row>
     <row r="326" ht="14.25" customHeight="1">
-      <c r="A326" s="43"/>
+      <c r="A326" s="37"/>
     </row>
     <row r="327" ht="14.25" customHeight="1">
-      <c r="A327" s="43"/>
+      <c r="A327" s="37"/>
     </row>
     <row r="328" ht="14.25" customHeight="1">
-      <c r="A328" s="43"/>
+      <c r="A328" s="37"/>
     </row>
     <row r="329" ht="14.25" customHeight="1">
-      <c r="A329" s="43"/>
+      <c r="A329" s="37"/>
     </row>
     <row r="330" ht="14.25" customHeight="1">
-      <c r="A330" s="43"/>
+      <c r="A330" s="37"/>
     </row>
     <row r="331" ht="14.25" customHeight="1">
-      <c r="A331" s="43"/>
+      <c r="A331" s="37"/>
     </row>
     <row r="332" ht="14.25" customHeight="1">
-      <c r="A332" s="43"/>
+      <c r="A332" s="37"/>
     </row>
     <row r="333" ht="14.25" customHeight="1">
-      <c r="A333" s="43"/>
+      <c r="A333" s="37"/>
     </row>
     <row r="334" ht="14.25" customHeight="1">
-      <c r="A334" s="43"/>
+      <c r="A334" s="37"/>
     </row>
     <row r="335" ht="14.25" customHeight="1">
-      <c r="A335" s="43"/>
+      <c r="A335" s="37"/>
     </row>
     <row r="336" ht="14.25" customHeight="1">
-      <c r="A336" s="43"/>
+      <c r="A336" s="37"/>
     </row>
     <row r="337" ht="14.25" customHeight="1">
-      <c r="A337" s="43"/>
+      <c r="A337" s="37"/>
     </row>
     <row r="338" ht="14.25" customHeight="1">
-      <c r="A338" s="43"/>
+      <c r="A338" s="37"/>
     </row>
     <row r="339" ht="14.25" customHeight="1">
-      <c r="A339" s="43"/>
+      <c r="A339" s="37"/>
     </row>
     <row r="340" ht="14.25" customHeight="1">
-      <c r="A340" s="43"/>
+      <c r="A340" s="37"/>
     </row>
     <row r="341" ht="14.25" customHeight="1">
-      <c r="A341" s="43"/>
+      <c r="A341" s="37"/>
     </row>
     <row r="342" ht="14.25" customHeight="1">
-      <c r="A342" s="43"/>
+      <c r="A342" s="37"/>
     </row>
     <row r="343" ht="14.25" customHeight="1">
-      <c r="A343" s="43"/>
+      <c r="A343" s="37"/>
     </row>
     <row r="344" ht="14.25" customHeight="1">
-      <c r="A344" s="43"/>
+      <c r="A344" s="37"/>
     </row>
     <row r="345" ht="14.25" customHeight="1">
-      <c r="A345" s="43"/>
+      <c r="A345" s="37"/>
     </row>
     <row r="346" ht="14.25" customHeight="1">
-      <c r="A346" s="43"/>
+      <c r="A346" s="37"/>
     </row>
     <row r="347" ht="14.25" customHeight="1">
-      <c r="A347" s="43"/>
+      <c r="A347" s="37"/>
     </row>
     <row r="348" ht="14.25" customHeight="1">
-      <c r="A348" s="43"/>
+      <c r="A348" s="37"/>
     </row>
     <row r="349" ht="14.25" customHeight="1">
-      <c r="A349" s="43"/>
+      <c r="A349" s="37"/>
     </row>
     <row r="350" ht="14.25" customHeight="1">
-      <c r="A350" s="43"/>
+      <c r="A350" s="37"/>
     </row>
     <row r="351" ht="14.25" customHeight="1">
-      <c r="A351" s="43"/>
+      <c r="A351" s="37"/>
     </row>
     <row r="352" ht="14.25" customHeight="1">
-      <c r="A352" s="43"/>
+      <c r="A352" s="37"/>
     </row>
     <row r="353" ht="14.25" customHeight="1">
-      <c r="A353" s="43"/>
+      <c r="A353" s="37"/>
     </row>
     <row r="354" ht="14.25" customHeight="1">
-      <c r="A354" s="43"/>
+      <c r="A354" s="37"/>
     </row>
     <row r="355" ht="14.25" customHeight="1">
-      <c r="A355" s="43"/>
+      <c r="A355" s="37"/>
     </row>
     <row r="356" ht="14.25" customHeight="1">
-      <c r="A356" s="43"/>
+      <c r="A356" s="37"/>
     </row>
     <row r="357" ht="14.25" customHeight="1">
-      <c r="A357" s="43"/>
+      <c r="A357" s="37"/>
     </row>
     <row r="358" ht="14.25" customHeight="1">
-      <c r="A358" s="43"/>
+      <c r="A358" s="37"/>
     </row>
     <row r="359" ht="14.25" customHeight="1">
-      <c r="A359" s="43"/>
+      <c r="A359" s="37"/>
     </row>
     <row r="360" ht="14.25" customHeight="1">
-      <c r="A360" s="43"/>
+      <c r="A360" s="37"/>
     </row>
     <row r="361" ht="14.25" customHeight="1">
-      <c r="A361" s="43"/>
+      <c r="A361" s="37"/>
     </row>
     <row r="362" ht="14.25" customHeight="1">
-      <c r="A362" s="43"/>
+      <c r="A362" s="37"/>
     </row>
     <row r="363" ht="14.25" customHeight="1">
-      <c r="A363" s="43"/>
+      <c r="A363" s="37"/>
     </row>
     <row r="364" ht="14.25" customHeight="1">
-      <c r="A364" s="43"/>
+      <c r="A364" s="37"/>
     </row>
     <row r="365" ht="14.25" customHeight="1">
-      <c r="A365" s="43"/>
+      <c r="A365" s="37"/>
     </row>
     <row r="366" ht="14.25" customHeight="1">
-      <c r="A366" s="43"/>
+      <c r="A366" s="37"/>
     </row>
     <row r="367" ht="14.25" customHeight="1">
-      <c r="A367" s="43"/>
+      <c r="A367" s="37"/>
     </row>
     <row r="368" ht="14.25" customHeight="1">
-      <c r="A368" s="43"/>
+      <c r="A368" s="37"/>
     </row>
     <row r="369" ht="14.25" customHeight="1">
-      <c r="A369" s="43"/>
+      <c r="A369" s="37"/>
     </row>
     <row r="370" ht="14.25" customHeight="1">
-      <c r="A370" s="43"/>
+      <c r="A370" s="37"/>
     </row>
     <row r="371" ht="14.25" customHeight="1">
-      <c r="A371" s="43"/>
+      <c r="A371" s="37"/>
     </row>
     <row r="372" ht="14.25" customHeight="1">
-      <c r="A372" s="43"/>
+      <c r="A372" s="37"/>
     </row>
     <row r="373" ht="14.25" customHeight="1">
-      <c r="A373" s="43"/>
+      <c r="A373" s="37"/>
     </row>
     <row r="374" ht="14.25" customHeight="1">
-      <c r="A374" s="43"/>
+      <c r="A374" s="37"/>
     </row>
     <row r="375" ht="14.25" customHeight="1">
-      <c r="A375" s="43"/>
+      <c r="A375" s="37"/>
     </row>
     <row r="376" ht="14.25" customHeight="1">
-      <c r="A376" s="43"/>
+      <c r="A376" s="37"/>
     </row>
     <row r="377" ht="14.25" customHeight="1">
-      <c r="A377" s="43"/>
+      <c r="A377" s="37"/>
     </row>
     <row r="378" ht="14.25" customHeight="1">
-      <c r="A378" s="43"/>
+      <c r="A378" s="37"/>
     </row>
     <row r="379" ht="14.25" customHeight="1">
-      <c r="A379" s="43"/>
+      <c r="A379" s="37"/>
     </row>
     <row r="380" ht="14.25" customHeight="1">
-      <c r="A380" s="43"/>
+      <c r="A380" s="37"/>
     </row>
     <row r="381" ht="14.25" customHeight="1">
-      <c r="A381" s="43"/>
+      <c r="A381" s="37"/>
     </row>
     <row r="382" ht="14.25" customHeight="1">
-      <c r="A382" s="43"/>
+      <c r="A382" s="37"/>
     </row>
     <row r="383" ht="14.25" customHeight="1">
-      <c r="A383" s="43"/>
+      <c r="A383" s="37"/>
     </row>
     <row r="384" ht="14.25" customHeight="1">
-      <c r="A384" s="43"/>
+      <c r="A384" s="37"/>
     </row>
     <row r="385" ht="14.25" customHeight="1">
-      <c r="A385" s="43"/>
+      <c r="A385" s="37"/>
     </row>
     <row r="386" ht="14.25" customHeight="1">
-      <c r="A386" s="43"/>
+      <c r="A386" s="37"/>
     </row>
     <row r="387" ht="14.25" customHeight="1">
-      <c r="A387" s="43"/>
+      <c r="A387" s="37"/>
     </row>
     <row r="388" ht="14.25" customHeight="1">
-      <c r="A388" s="43"/>
+      <c r="A388" s="37"/>
     </row>
     <row r="389" ht="14.25" customHeight="1">
-      <c r="A389" s="43"/>
+      <c r="A389" s="37"/>
     </row>
     <row r="390" ht="14.25" customHeight="1">
-      <c r="A390" s="43"/>
+      <c r="A390" s="37"/>
     </row>
     <row r="391" ht="14.25" customHeight="1">
-      <c r="A391" s="43"/>
+      <c r="A391" s="37"/>
     </row>
     <row r="392" ht="14.25" customHeight="1">
-      <c r="A392" s="43"/>
+      <c r="A392" s="37"/>
     </row>
     <row r="393" ht="14.25" customHeight="1">
-      <c r="A393" s="43"/>
+      <c r="A393" s="37"/>
     </row>
     <row r="394" ht="14.25" customHeight="1">
-      <c r="A394" s="43"/>
+      <c r="A394" s="37"/>
     </row>
     <row r="395" ht="14.25" customHeight="1">
-      <c r="A395" s="43"/>
+      <c r="A395" s="37"/>
     </row>
     <row r="396" ht="14.25" customHeight="1">
-      <c r="A396" s="43"/>
+      <c r="A396" s="37"/>
     </row>
     <row r="397" ht="14.25" customHeight="1">
-      <c r="A397" s="43"/>
+      <c r="A397" s="37"/>
     </row>
     <row r="398" ht="14.25" customHeight="1">
-      <c r="A398" s="43"/>
+      <c r="A398" s="37"/>
     </row>
     <row r="399" ht="14.25" customHeight="1">
-      <c r="A399" s="43"/>
+      <c r="A399" s="37"/>
     </row>
     <row r="400" ht="14.25" customHeight="1">
-      <c r="A400" s="43"/>
+      <c r="A400" s="37"/>
     </row>
     <row r="401" ht="14.25" customHeight="1">
-      <c r="A401" s="43"/>
+      <c r="A401" s="37"/>
     </row>
     <row r="402" ht="14.25" customHeight="1">
-      <c r="A402" s="43"/>
+      <c r="A402" s="37"/>
     </row>
     <row r="403" ht="14.25" customHeight="1">
-      <c r="A403" s="43"/>
+      <c r="A403" s="37"/>
     </row>
     <row r="404" ht="14.25" customHeight="1">
-      <c r="A404" s="43"/>
+      <c r="A404" s="37"/>
     </row>
     <row r="405" ht="14.25" customHeight="1">
-      <c r="A405" s="43"/>
+      <c r="A405" s="37"/>
     </row>
     <row r="406" ht="14.25" customHeight="1">
-      <c r="A406" s="43"/>
+      <c r="A406" s="37"/>
     </row>
     <row r="407" ht="14.25" customHeight="1">
-      <c r="A407" s="43"/>
+      <c r="A407" s="37"/>
     </row>
     <row r="408" ht="14.25" customHeight="1">
-      <c r="A408" s="43"/>
+      <c r="A408" s="37"/>
     </row>
     <row r="409" ht="14.25" customHeight="1">
-      <c r="A409" s="43"/>
+      <c r="A409" s="37"/>
     </row>
     <row r="410" ht="14.25" customHeight="1">
-      <c r="A410" s="43"/>
+      <c r="A410" s="37"/>
     </row>
     <row r="411" ht="14.25" customHeight="1">
-      <c r="A411" s="43"/>
+      <c r="A411" s="37"/>
     </row>
     <row r="412" ht="14.25" customHeight="1">
-      <c r="A412" s="43"/>
+      <c r="A412" s="37"/>
     </row>
     <row r="413" ht="14.25" customHeight="1">
-      <c r="A413" s="43"/>
+      <c r="A413" s="37"/>
     </row>
     <row r="414" ht="14.25" customHeight="1">
-      <c r="A414" s="43"/>
+      <c r="A414" s="37"/>
     </row>
     <row r="415" ht="14.25" customHeight="1">
-      <c r="A415" s="43"/>
+      <c r="A415" s="37"/>
     </row>
     <row r="416" ht="14.25" customHeight="1">
-      <c r="A416" s="43"/>
+      <c r="A416" s="37"/>
     </row>
     <row r="417" ht="14.25" customHeight="1">
-      <c r="A417" s="43"/>
+      <c r="A417" s="37"/>
     </row>
     <row r="418" ht="14.25" customHeight="1">
-      <c r="A418" s="43"/>
+      <c r="A418" s="37"/>
     </row>
     <row r="419" ht="14.25" customHeight="1">
-      <c r="A419" s="43"/>
+      <c r="A419" s="37"/>
     </row>
     <row r="420" ht="14.25" customHeight="1">
-      <c r="A420" s="43"/>
+      <c r="A420" s="37"/>
     </row>
     <row r="421" ht="14.25" customHeight="1">
-      <c r="A421" s="43"/>
+      <c r="A421" s="37"/>
     </row>
     <row r="422" ht="14.25" customHeight="1">
-      <c r="A422" s="43"/>
+      <c r="A422" s="37"/>
     </row>
     <row r="423" ht="14.25" customHeight="1">
-      <c r="A423" s="43"/>
+      <c r="A423" s="37"/>
     </row>
     <row r="424" ht="14.25" customHeight="1">
-      <c r="A424" s="43"/>
+      <c r="A424" s="37"/>
     </row>
     <row r="425" ht="14.25" customHeight="1">
-      <c r="A425" s="43"/>
+      <c r="A425" s="37"/>
     </row>
     <row r="426" ht="14.25" customHeight="1">
-      <c r="A426" s="43"/>
+      <c r="A426" s="37"/>
     </row>
     <row r="427" ht="14.25" customHeight="1">
-      <c r="A427" s="43"/>
+      <c r="A427" s="37"/>
     </row>
     <row r="428" ht="14.25" customHeight="1">
-      <c r="A428" s="43"/>
+      <c r="A428" s="37"/>
     </row>
     <row r="429" ht="14.25" customHeight="1">
-      <c r="A429" s="43"/>
+      <c r="A429" s="37"/>
     </row>
     <row r="430" ht="14.25" customHeight="1">
-      <c r="A430" s="43"/>
+      <c r="A430" s="37"/>
     </row>
     <row r="431" ht="14.25" customHeight="1">
-      <c r="A431" s="43"/>
+      <c r="A431" s="37"/>
     </row>
     <row r="432" ht="14.25" customHeight="1">
-      <c r="A432" s="43"/>
+      <c r="A432" s="37"/>
     </row>
     <row r="433" ht="14.25" customHeight="1">
-      <c r="A433" s="43"/>
+      <c r="A433" s="37"/>
     </row>
     <row r="434" ht="14.25" customHeight="1">
-      <c r="A434" s="43"/>
+      <c r="A434" s="37"/>
     </row>
     <row r="435" ht="14.25" customHeight="1">
-      <c r="A435" s="43"/>
+      <c r="A435" s="37"/>
     </row>
     <row r="436" ht="14.25" customHeight="1">
-      <c r="A436" s="43"/>
+      <c r="A436" s="37"/>
     </row>
     <row r="437" ht="14.25" customHeight="1">
-      <c r="A437" s="43"/>
+      <c r="A437" s="37"/>
     </row>
     <row r="438" ht="14.25" customHeight="1">
-      <c r="A438" s="43"/>
+      <c r="A438" s="37"/>
     </row>
     <row r="439" ht="14.25" customHeight="1">
-      <c r="A439" s="43"/>
+      <c r="A439" s="37"/>
     </row>
     <row r="440" ht="14.25" customHeight="1">
-      <c r="A440" s="43"/>
+      <c r="A440" s="37"/>
     </row>
     <row r="441" ht="14.25" customHeight="1">
-      <c r="A441" s="43"/>
+      <c r="A441" s="37"/>
     </row>
     <row r="442" ht="14.25" customHeight="1">
-      <c r="A442" s="43"/>
+      <c r="A442" s="37"/>
     </row>
     <row r="443" ht="14.25" customHeight="1">
-      <c r="A443" s="43"/>
+      <c r="A443" s="37"/>
     </row>
     <row r="444" ht="14.25" customHeight="1">
-      <c r="A444" s="43"/>
+      <c r="A444" s="37"/>
     </row>
     <row r="445" ht="14.25" customHeight="1">
-      <c r="A445" s="43"/>
+      <c r="A445" s="37"/>
     </row>
     <row r="446" ht="14.25" customHeight="1">
-      <c r="A446" s="43"/>
+      <c r="A446" s="37"/>
     </row>
     <row r="447" ht="14.25" customHeight="1">
-      <c r="A447" s="43"/>
+      <c r="A447" s="37"/>
     </row>
     <row r="448" ht="14.25" customHeight="1">
-      <c r="A448" s="43"/>
+      <c r="A448" s="37"/>
     </row>
     <row r="449" ht="14.25" customHeight="1">
-      <c r="A449" s="43"/>
+      <c r="A449" s="37"/>
     </row>
     <row r="450" ht="14.25" customHeight="1">
-      <c r="A450" s="43"/>
+      <c r="A450" s="37"/>
     </row>
     <row r="451" ht="14.25" customHeight="1">
-      <c r="A451" s="43"/>
+      <c r="A451" s="37"/>
     </row>
     <row r="452" ht="14.25" customHeight="1">
-      <c r="A452" s="43"/>
+      <c r="A452" s="37"/>
     </row>
     <row r="453" ht="14.25" customHeight="1">
-      <c r="A453" s="43"/>
+      <c r="A453" s="37"/>
     </row>
     <row r="454" ht="14.25" customHeight="1">
-      <c r="A454" s="43"/>
+      <c r="A454" s="37"/>
     </row>
     <row r="455" ht="14.25" customHeight="1">
-      <c r="A455" s="43"/>
+      <c r="A455" s="37"/>
     </row>
     <row r="456" ht="14.25" customHeight="1">
-      <c r="A456" s="43"/>
+      <c r="A456" s="37"/>
     </row>
     <row r="457" ht="14.25" customHeight="1">
-      <c r="A457" s="43"/>
+      <c r="A457" s="37"/>
     </row>
     <row r="458" ht="14.25" customHeight="1">
-      <c r="A458" s="43"/>
+      <c r="A458" s="37"/>
     </row>
     <row r="459" ht="14.25" customHeight="1">
-      <c r="A459" s="43"/>
+      <c r="A459" s="37"/>
     </row>
     <row r="460" ht="14.25" customHeight="1">
-      <c r="A460" s="43"/>
+      <c r="A460" s="37"/>
     </row>
     <row r="461" ht="14.25" customHeight="1">
-      <c r="A461" s="43"/>
+      <c r="A461" s="37"/>
     </row>
     <row r="462" ht="14.25" customHeight="1">
-      <c r="A462" s="43"/>
+      <c r="A462" s="37"/>
     </row>
     <row r="463" ht="14.25" customHeight="1">
-      <c r="A463" s="43"/>
+      <c r="A463" s="37"/>
     </row>
     <row r="464" ht="14.25" customHeight="1">
-      <c r="A464" s="43"/>
+      <c r="A464" s="37"/>
     </row>
     <row r="465" ht="14.25" customHeight="1">
-      <c r="A465" s="43"/>
+      <c r="A465" s="37"/>
     </row>
     <row r="466" ht="14.25" customHeight="1">
-      <c r="A466" s="43"/>
+      <c r="A466" s="37"/>
     </row>
     <row r="467" ht="14.25" customHeight="1">
-      <c r="A467" s="43"/>
+      <c r="A467" s="37"/>
     </row>
     <row r="468" ht="14.25" customHeight="1">
-      <c r="A468" s="43"/>
+      <c r="A468" s="37"/>
     </row>
     <row r="469" ht="14.25" customHeight="1">
-      <c r="A469" s="43"/>
+      <c r="A469" s="37"/>
     </row>
     <row r="470" ht="14.25" customHeight="1">
-      <c r="A470" s="43"/>
+      <c r="A470" s="37"/>
     </row>
     <row r="471" ht="14.25" customHeight="1">
-      <c r="A471" s="43"/>
+      <c r="A471" s="37"/>
     </row>
     <row r="472" ht="14.25" customHeight="1">
-      <c r="A472" s="43"/>
+      <c r="A472" s="37"/>
     </row>
     <row r="473" ht="14.25" customHeight="1">
-      <c r="A473" s="43"/>
+      <c r="A473" s="37"/>
     </row>
     <row r="474" ht="14.25" customHeight="1">
-      <c r="A474" s="43"/>
+      <c r="A474" s="37"/>
     </row>
     <row r="475" ht="14.25" customHeight="1">
-      <c r="A475" s="43"/>
+      <c r="A475" s="37"/>
     </row>
     <row r="476" ht="14.25" customHeight="1">
-      <c r="A476" s="43"/>
+      <c r="A476" s="37"/>
     </row>
     <row r="477" ht="14.25" customHeight="1">
-      <c r="A477" s="43"/>
+      <c r="A477" s="37"/>
     </row>
     <row r="478" ht="14.25" customHeight="1">
-      <c r="A478" s="43"/>
+      <c r="A478" s="37"/>
     </row>
     <row r="479" ht="14.25" customHeight="1">
-      <c r="A479" s="43"/>
+      <c r="A479" s="37"/>
     </row>
     <row r="480" ht="14.25" customHeight="1">
-      <c r="A480" s="43"/>
+      <c r="A480" s="37"/>
     </row>
     <row r="481" ht="14.25" customHeight="1">
-      <c r="A481" s="43"/>
+      <c r="A481" s="37"/>
     </row>
     <row r="482" ht="14.25" customHeight="1">
-      <c r="A482" s="43"/>
+      <c r="A482" s="37"/>
     </row>
     <row r="483" ht="14.25" customHeight="1">
-      <c r="A483" s="43"/>
+      <c r="A483" s="37"/>
     </row>
     <row r="484" ht="14.25" customHeight="1">
-      <c r="A484" s="43"/>
+      <c r="A484" s="37"/>
     </row>
     <row r="485" ht="14.25" customHeight="1">
-      <c r="A485" s="43"/>
+      <c r="A485" s="37"/>
     </row>
     <row r="486" ht="14.25" customHeight="1">
-      <c r="A486" s="43"/>
+      <c r="A486" s="37"/>
     </row>
     <row r="487" ht="14.25" customHeight="1">
-      <c r="A487" s="43"/>
+      <c r="A487" s="37"/>
     </row>
     <row r="488" ht="14.25" customHeight="1">
-      <c r="A488" s="43"/>
+      <c r="A488" s="37"/>
     </row>
     <row r="489" ht="14.25" customHeight="1">
-      <c r="A489" s="43"/>
+      <c r="A489" s="37"/>
     </row>
     <row r="490" ht="14.25" customHeight="1">
-      <c r="A490" s="43"/>
+      <c r="A490" s="37"/>
     </row>
     <row r="491" ht="14.25" customHeight="1">
-      <c r="A491" s="43"/>
+      <c r="A491" s="37"/>
     </row>
     <row r="492" ht="14.25" customHeight="1">
-      <c r="A492" s="43"/>
+      <c r="A492" s="37"/>
     </row>
     <row r="493" ht="14.25" customHeight="1">
-      <c r="A493" s="43"/>
+      <c r="A493" s="37"/>
     </row>
     <row r="494" ht="14.25" customHeight="1">
-      <c r="A494" s="43"/>
+      <c r="A494" s="37"/>
     </row>
     <row r="495" ht="14.25" customHeight="1">
-      <c r="A495" s="43"/>
+      <c r="A495" s="37"/>
     </row>
     <row r="496" ht="14.25" customHeight="1">
-      <c r="A496" s="43"/>
+      <c r="A496" s="37"/>
     </row>
     <row r="497" ht="14.25" customHeight="1">
-      <c r="A497" s="43"/>
+      <c r="A497" s="37"/>
     </row>
     <row r="498" ht="14.25" customHeight="1">
-      <c r="A498" s="43"/>
+      <c r="A498" s="37"/>
     </row>
     <row r="499" ht="14.25" customHeight="1">
-      <c r="A499" s="43"/>
+      <c r="A499" s="37"/>
     </row>
     <row r="500" ht="14.25" customHeight="1">
-      <c r="A500" s="43"/>
+      <c r="A500" s="37"/>
     </row>
     <row r="501" ht="14.25" customHeight="1">
-      <c r="A501" s="43"/>
+      <c r="A501" s="37"/>
     </row>
     <row r="502" ht="14.25" customHeight="1">
-      <c r="A502" s="43"/>
+      <c r="A502" s="37"/>
     </row>
     <row r="503" ht="14.25" customHeight="1">
-      <c r="A503" s="43"/>
+      <c r="A503" s="37"/>
     </row>
     <row r="504" ht="14.25" customHeight="1">
-      <c r="A504" s="43"/>
+      <c r="A504" s="37"/>
     </row>
     <row r="505" ht="14.25" customHeight="1">
-      <c r="A505" s="43"/>
+      <c r="A505" s="37"/>
     </row>
     <row r="506" ht="14.25" customHeight="1">
-      <c r="A506" s="43"/>
+      <c r="A506" s="37"/>
     </row>
     <row r="507" ht="14.25" customHeight="1">
-      <c r="A507" s="43"/>
+      <c r="A507" s="37"/>
     </row>
     <row r="508" ht="14.25" customHeight="1">
-      <c r="A508" s="43"/>
+      <c r="A508" s="37"/>
     </row>
     <row r="509" ht="14.25" customHeight="1">
-      <c r="A509" s="43"/>
+      <c r="A509" s="37"/>
     </row>
     <row r="510" ht="14.25" customHeight="1">
-      <c r="A510" s="43"/>
+      <c r="A510" s="37"/>
     </row>
     <row r="511" ht="14.25" customHeight="1">
-      <c r="A511" s="43"/>
+      <c r="A511" s="37"/>
     </row>
     <row r="512" ht="14.25" customHeight="1">
-      <c r="A512" s="43"/>
+      <c r="A512" s="37"/>
     </row>
     <row r="513" ht="14.25" customHeight="1">
-      <c r="A513" s="43"/>
+      <c r="A513" s="37"/>
     </row>
     <row r="514" ht="14.25" customHeight="1">
-      <c r="A514" s="43"/>
+      <c r="A514" s="37"/>
     </row>
     <row r="515" ht="14.25" customHeight="1">
-      <c r="A515" s="43"/>
+      <c r="A515" s="37"/>
     </row>
     <row r="516" ht="14.25" customHeight="1">
-      <c r="A516" s="43"/>
+      <c r="A516" s="37"/>
     </row>
     <row r="517" ht="14.25" customHeight="1">
-      <c r="A517" s="43"/>
+      <c r="A517" s="37"/>
     </row>
     <row r="518" ht="14.25" customHeight="1">
-      <c r="A518" s="43"/>
+      <c r="A518" s="37"/>
     </row>
     <row r="519" ht="14.25" customHeight="1">
-      <c r="A519" s="43"/>
+      <c r="A519" s="37"/>
     </row>
     <row r="520" ht="14.25" customHeight="1">
-      <c r="A520" s="43"/>
+      <c r="A520" s="37"/>
     </row>
     <row r="521" ht="14.25" customHeight="1">
-      <c r="A521" s="43"/>
+      <c r="A521" s="37"/>
     </row>
     <row r="522" ht="14.25" customHeight="1">
-      <c r="A522" s="43"/>
+      <c r="A522" s="37"/>
     </row>
     <row r="523" ht="14.25" customHeight="1">
-      <c r="A523" s="43"/>
+      <c r="A523" s="37"/>
     </row>
     <row r="524" ht="14.25" customHeight="1">
-      <c r="A524" s="43"/>
+      <c r="A524" s="37"/>
     </row>
     <row r="525" ht="14.25" customHeight="1">
-      <c r="A525" s="43"/>
+      <c r="A525" s="37"/>
     </row>
     <row r="526" ht="14.25" customHeight="1">
-      <c r="A526" s="43"/>
+      <c r="A526" s="37"/>
     </row>
     <row r="527" ht="14.25" customHeight="1">
-      <c r="A527" s="43"/>
+      <c r="A527" s="37"/>
     </row>
     <row r="528" ht="14.25" customHeight="1">
-      <c r="A528" s="43"/>
+      <c r="A528" s="37"/>
     </row>
     <row r="529" ht="14.25" customHeight="1">
-      <c r="A529" s="43"/>
+      <c r="A529" s="37"/>
     </row>
     <row r="530" ht="14.25" customHeight="1">
-      <c r="A530" s="43"/>
+      <c r="A530" s="37"/>
     </row>
     <row r="531" ht="14.25" customHeight="1">
-      <c r="A531" s="43"/>
+      <c r="A531" s="37"/>
     </row>
     <row r="532" ht="14.25" customHeight="1">
-      <c r="A532" s="43"/>
+      <c r="A532" s="37"/>
     </row>
     <row r="533" ht="14.25" customHeight="1">
-      <c r="A533" s="43"/>
+      <c r="A533" s="37"/>
     </row>
     <row r="534" ht="14.25" customHeight="1">
-      <c r="A534" s="43"/>
+      <c r="A534" s="37"/>
     </row>
     <row r="535" ht="14.25" customHeight="1">
-      <c r="A535" s="43"/>
+      <c r="A535" s="37"/>
     </row>
     <row r="536" ht="14.25" customHeight="1">
-      <c r="A536" s="43"/>
+      <c r="A536" s="37"/>
     </row>
     <row r="537" ht="14.25" customHeight="1">
-      <c r="A537" s="43"/>
+      <c r="A537" s="37"/>
     </row>
     <row r="538" ht="14.25" customHeight="1">
-      <c r="A538" s="43"/>
+      <c r="A538" s="37"/>
     </row>
     <row r="539" ht="14.25" customHeight="1">
-      <c r="A539" s="43"/>
+      <c r="A539" s="37"/>
     </row>
     <row r="540" ht="14.25" customHeight="1">
-      <c r="A540" s="43"/>
+      <c r="A540" s="37"/>
     </row>
     <row r="541" ht="14.25" customHeight="1">
-      <c r="A541" s="43"/>
+      <c r="A541" s="37"/>
     </row>
     <row r="542" ht="14.25" customHeight="1">
-      <c r="A542" s="43"/>
+      <c r="A542" s="37"/>
     </row>
     <row r="543" ht="14.25" customHeight="1">
-      <c r="A543" s="43"/>
+      <c r="A543" s="37"/>
     </row>
     <row r="544" ht="14.25" customHeight="1">
-      <c r="A544" s="43"/>
+      <c r="A544" s="37"/>
     </row>
     <row r="545" ht="14.25" customHeight="1">
-      <c r="A545" s="43"/>
+      <c r="A545" s="37"/>
     </row>
     <row r="546" ht="14.25" customHeight="1">
-      <c r="A546" s="43"/>
+      <c r="A546" s="37"/>
     </row>
     <row r="547" ht="14.25" customHeight="1">
-      <c r="A547" s="43"/>
+      <c r="A547" s="37"/>
     </row>
     <row r="548" ht="14.25" customHeight="1">
-      <c r="A548" s="43"/>
+      <c r="A548" s="37"/>
     </row>
     <row r="549" ht="14.25" customHeight="1">
-      <c r="A549" s="43"/>
+      <c r="A549" s="37"/>
     </row>
     <row r="550" ht="14.25" customHeight="1">
-      <c r="A550" s="43"/>
+      <c r="A550" s="37"/>
     </row>
     <row r="551" ht="14.25" customHeight="1">
-      <c r="A551" s="43"/>
+      <c r="A551" s="37"/>
     </row>
     <row r="552" ht="14.25" customHeight="1">
-      <c r="A552" s="43"/>
+      <c r="A552" s="37"/>
     </row>
     <row r="553" ht="14.25" customHeight="1">
-      <c r="A553" s="43"/>
+      <c r="A553" s="37"/>
     </row>
     <row r="554" ht="14.25" customHeight="1">
-      <c r="A554" s="43"/>
+      <c r="A554" s="37"/>
     </row>
     <row r="555" ht="14.25" customHeight="1">
-      <c r="A555" s="43"/>
+      <c r="A555" s="37"/>
     </row>
     <row r="556" ht="14.25" customHeight="1">
-      <c r="A556" s="43"/>
+      <c r="A556" s="37"/>
     </row>
     <row r="557" ht="14.25" customHeight="1">
-      <c r="A557" s="43"/>
+      <c r="A557" s="37"/>
     </row>
     <row r="558" ht="14.25" customHeight="1">
-      <c r="A558" s="43"/>
+      <c r="A558" s="37"/>
     </row>
     <row r="559" ht="14.25" customHeight="1">
-      <c r="A559" s="43"/>
+      <c r="A559" s="37"/>
     </row>
     <row r="560" ht="14.25" customHeight="1">
-      <c r="A560" s="43"/>
+      <c r="A560" s="37"/>
     </row>
     <row r="561" ht="14.25" customHeight="1">
-      <c r="A561" s="43"/>
+      <c r="A561" s="37"/>
     </row>
     <row r="562" ht="14.25" customHeight="1">
-      <c r="A562" s="43"/>
+      <c r="A562" s="37"/>
     </row>
     <row r="563" ht="14.25" customHeight="1">
-      <c r="A563" s="43"/>
+      <c r="A563" s="37"/>
     </row>
     <row r="564" ht="14.25" customHeight="1">
-      <c r="A564" s="43"/>
+      <c r="A564" s="37"/>
     </row>
     <row r="565" ht="14.25" customHeight="1">
-      <c r="A565" s="43"/>
+      <c r="A565" s="37"/>
     </row>
     <row r="566" ht="14.25" customHeight="1">
-      <c r="A566" s="43"/>
+      <c r="A566" s="37"/>
     </row>
     <row r="567" ht="14.25" customHeight="1">
-      <c r="A567" s="43"/>
+      <c r="A567" s="37"/>
     </row>
     <row r="568" ht="14.25" customHeight="1">
-      <c r="A568" s="43"/>
+      <c r="A568" s="37"/>
     </row>
     <row r="569" ht="14.25" customHeight="1">
-      <c r="A569" s="43"/>
+      <c r="A569" s="37"/>
     </row>
     <row r="570" ht="14.25" customHeight="1">
-      <c r="A570" s="43"/>
+      <c r="A570" s="37"/>
     </row>
     <row r="571" ht="14.25" customHeight="1">
-      <c r="A571" s="43"/>
+      <c r="A571" s="37"/>
     </row>
     <row r="572" ht="14.25" customHeight="1">
-      <c r="A572" s="43"/>
+      <c r="A572" s="37"/>
     </row>
     <row r="573" ht="14.25" customHeight="1">
-      <c r="A573" s="43"/>
+      <c r="A573" s="37"/>
     </row>
     <row r="574" ht="14.25" customHeight="1">
-      <c r="A574" s="43"/>
+      <c r="A574" s="37"/>
     </row>
     <row r="575" ht="14.25" customHeight="1">
-      <c r="A575" s="43"/>
+      <c r="A575" s="37"/>
     </row>
     <row r="576" ht="14.25" customHeight="1">
-      <c r="A576" s="43"/>
+      <c r="A576" s="37"/>
     </row>
     <row r="577" ht="14.25" customHeight="1">
-      <c r="A577" s="43"/>
+      <c r="A577" s="37"/>
     </row>
     <row r="578" ht="14.25" customHeight="1">
-      <c r="A578" s="43"/>
+      <c r="A578" s="37"/>
     </row>
     <row r="579" ht="14.25" customHeight="1">
-      <c r="A579" s="43"/>
+      <c r="A579" s="37"/>
     </row>
     <row r="580" ht="14.25" customHeight="1">
-      <c r="A580" s="43"/>
+      <c r="A580" s="37"/>
     </row>
     <row r="581" ht="14.25" customHeight="1">
-      <c r="A581" s="43"/>
+      <c r="A581" s="37"/>
     </row>
     <row r="582" ht="14.25" customHeight="1">
-      <c r="A582" s="43"/>
+      <c r="A582" s="37"/>
     </row>
     <row r="583" ht="14.25" customHeight="1">
-      <c r="A583" s="43"/>
+      <c r="A583" s="37"/>
     </row>
     <row r="584" ht="14.25" customHeight="1">
-      <c r="A584" s="43"/>
+      <c r="A584" s="37"/>
     </row>
     <row r="585" ht="14.25" customHeight="1">
-      <c r="A585" s="43"/>
+      <c r="A585" s="37"/>
     </row>
     <row r="586" ht="14.25" customHeight="1">
-      <c r="A586" s="43"/>
+      <c r="A586" s="37"/>
     </row>
     <row r="587" ht="14.25" customHeight="1">
-      <c r="A587" s="43"/>
+      <c r="A587" s="37"/>
     </row>
     <row r="588" ht="14.25" customHeight="1">
-      <c r="A588" s="43"/>
+      <c r="A588" s="37"/>
     </row>
     <row r="589" ht="14.25" customHeight="1">
-      <c r="A589" s="43"/>
+      <c r="A589" s="37"/>
     </row>
     <row r="590" ht="14.25" customHeight="1">
-      <c r="A590" s="43"/>
+      <c r="A590" s="37"/>
     </row>
     <row r="591" ht="14.25" customHeight="1">
-      <c r="A591" s="43"/>
+      <c r="A591" s="37"/>
     </row>
     <row r="592" ht="14.25" customHeight="1">
-      <c r="A592" s="43"/>
+      <c r="A592" s="37"/>
     </row>
     <row r="593" ht="14.25" customHeight="1">
-      <c r="A593" s="43"/>
+      <c r="A593" s="37"/>
     </row>
     <row r="594" ht="14.25" customHeight="1">
-      <c r="A594" s="43"/>
+      <c r="A594" s="37"/>
     </row>
     <row r="595" ht="14.25" customHeight="1">
-      <c r="A595" s="43"/>
+      <c r="A595" s="37"/>
     </row>
     <row r="596" ht="14.25" customHeight="1">
-      <c r="A596" s="43"/>
+      <c r="A596" s="37"/>
     </row>
     <row r="597" ht="14.25" customHeight="1">
-      <c r="A597" s="43"/>
+      <c r="A597" s="37"/>
     </row>
     <row r="598" ht="14.25" customHeight="1">
-      <c r="A598" s="43"/>
+      <c r="A598" s="37"/>
     </row>
     <row r="599" ht="14.25" customHeight="1">
-      <c r="A599" s="43"/>
+      <c r="A599" s="37"/>
     </row>
     <row r="600" ht="14.25" customHeight="1">
-      <c r="A600" s="43"/>
+      <c r="A600" s="37"/>
     </row>
     <row r="601" ht="14.25" customHeight="1">
-      <c r="A601" s="43"/>
+      <c r="A601" s="37"/>
     </row>
     <row r="602" ht="14.25" customHeight="1">
-      <c r="A602" s="43"/>
+      <c r="A602" s="37"/>
     </row>
     <row r="603" ht="14.25" customHeight="1">
-      <c r="A603" s="43"/>
+      <c r="A603" s="37"/>
     </row>
     <row r="604" ht="14.25" customHeight="1">
-      <c r="A604" s="43"/>
+      <c r="A604" s="37"/>
     </row>
     <row r="605" ht="14.25" customHeight="1">
-      <c r="A605" s="43"/>
+      <c r="A605" s="37"/>
     </row>
     <row r="606" ht="14.25" customHeight="1">
-      <c r="A606" s="43"/>
+      <c r="A606" s="37"/>
     </row>
     <row r="607" ht="14.25" customHeight="1">
-      <c r="A607" s="43"/>
+      <c r="A607" s="37"/>
     </row>
     <row r="608" ht="14.25" customHeight="1">
-      <c r="A608" s="43"/>
+      <c r="A608" s="37"/>
     </row>
     <row r="609" ht="14.25" customHeight="1">
-      <c r="A609" s="43"/>
+      <c r="A609" s="37"/>
     </row>
     <row r="610" ht="14.25" customHeight="1">
-      <c r="A610" s="43"/>
+      <c r="A610" s="37"/>
     </row>
     <row r="611" ht="14.25" customHeight="1">
-      <c r="A611" s="43"/>
+      <c r="A611" s="37"/>
     </row>
     <row r="612" ht="14.25" customHeight="1">
-      <c r="A612" s="43"/>
+      <c r="A612" s="37"/>
     </row>
     <row r="613" ht="14.25" customHeight="1">
-      <c r="A613" s="43"/>
+      <c r="A613" s="37"/>
     </row>
     <row r="614" ht="14.25" customHeight="1">
-      <c r="A614" s="43"/>
+      <c r="A614" s="37"/>
     </row>
     <row r="615" ht="14.25" customHeight="1">
-      <c r="A615" s="43"/>
+      <c r="A615" s="37"/>
     </row>
     <row r="616" ht="14.25" customHeight="1">
-      <c r="A616" s="43"/>
+      <c r="A616" s="37"/>
     </row>
     <row r="617" ht="14.25" customHeight="1">
-      <c r="A617" s="43"/>
+      <c r="A617" s="37"/>
     </row>
     <row r="618" ht="14.25" customHeight="1">
-      <c r="A618" s="43"/>
+      <c r="A618" s="37"/>
     </row>
     <row r="619" ht="14.25" customHeight="1">
-      <c r="A619" s="43"/>
+      <c r="A619" s="37"/>
     </row>
     <row r="620" ht="14.25" customHeight="1">
-      <c r="A620" s="43"/>
+      <c r="A620" s="37"/>
     </row>
     <row r="621" ht="14.25" customHeight="1">
-      <c r="A621" s="43"/>
+      <c r="A621" s="37"/>
     </row>
     <row r="622" ht="14.25" customHeight="1">
-      <c r="A622" s="43"/>
+      <c r="A622" s="37"/>
     </row>
     <row r="623" ht="14.25" customHeight="1">
-      <c r="A623" s="43"/>
+      <c r="A623" s="37"/>
     </row>
     <row r="624" ht="14.25" customHeight="1">
-      <c r="A624" s="43"/>
+      <c r="A624" s="37"/>
     </row>
     <row r="625" ht="14.25" customHeight="1">
-      <c r="A625" s="43"/>
+      <c r="A625" s="37"/>
     </row>
     <row r="626" ht="14.25" customHeight="1">
-      <c r="A626" s="43"/>
+      <c r="A626" s="37"/>
     </row>
     <row r="627" ht="14.25" customHeight="1">
-      <c r="A627" s="43"/>
+      <c r="A627" s="37"/>
     </row>
     <row r="628" ht="14.25" customHeight="1">
-      <c r="A628" s="43"/>
+      <c r="A628" s="37"/>
     </row>
     <row r="629" ht="14.25" customHeight="1">
-      <c r="A629" s="43"/>
+      <c r="A629" s="37"/>
     </row>
     <row r="630" ht="14.25" customHeight="1">
-      <c r="A630" s="43"/>
+      <c r="A630" s="37"/>
     </row>
     <row r="631" ht="14.25" customHeight="1">
-      <c r="A631" s="43"/>
+      <c r="A631" s="37"/>
     </row>
     <row r="632" ht="14.25" customHeight="1">
-      <c r="A632" s="43"/>
+      <c r="A632" s="37"/>
     </row>
     <row r="633" ht="14.25" customHeight="1">
-      <c r="A633" s="43"/>
+      <c r="A633" s="37"/>
     </row>
     <row r="634" ht="14.25" customHeight="1">
-      <c r="A634" s="43"/>
+      <c r="A634" s="37"/>
     </row>
     <row r="635" ht="14.25" customHeight="1">
-      <c r="A635" s="43"/>
+      <c r="A635" s="37"/>
     </row>
     <row r="636" ht="14.25" customHeight="1">
-      <c r="A636" s="43"/>
+      <c r="A636" s="37"/>
     </row>
     <row r="637" ht="14.25" customHeight="1">
-      <c r="A637" s="43"/>
+      <c r="A637" s="37"/>
     </row>
     <row r="638" ht="14.25" customHeight="1">
-      <c r="A638" s="43"/>
+      <c r="A638" s="37"/>
     </row>
     <row r="639" ht="14.25" customHeight="1">
-      <c r="A639" s="43"/>
+      <c r="A639" s="37"/>
     </row>
     <row r="640" ht="14.25" customHeight="1">
-      <c r="A640" s="43"/>
+      <c r="A640" s="37"/>
     </row>
     <row r="641" ht="14.25" customHeight="1">
-      <c r="A641" s="43"/>
+      <c r="A641" s="37"/>
     </row>
     <row r="642" ht="14.25" customHeight="1">
-      <c r="A642" s="43"/>
+      <c r="A642" s="37"/>
     </row>
     <row r="643" ht="14.25" customHeight="1">
-      <c r="A643" s="43"/>
+      <c r="A643" s="37"/>
     </row>
     <row r="644" ht="14.25" customHeight="1">
-      <c r="A644" s="43"/>
+      <c r="A644" s="37"/>
     </row>
     <row r="645" ht="14.25" customHeight="1">
-      <c r="A645" s="43"/>
+      <c r="A645" s="37"/>
     </row>
     <row r="646" ht="14.25" customHeight="1">
-      <c r="A646" s="43"/>
+      <c r="A646" s="37"/>
     </row>
     <row r="647" ht="14.25" customHeight="1">
-      <c r="A647" s="43"/>
+      <c r="A647" s="37"/>
     </row>
     <row r="648" ht="14.25" customHeight="1">
-      <c r="A648" s="43"/>
+      <c r="A648" s="37"/>
     </row>
     <row r="649" ht="14.25" customHeight="1">
-      <c r="A649" s="43"/>
+      <c r="A649" s="37"/>
     </row>
     <row r="650" ht="14.25" customHeight="1">
-      <c r="A650" s="43"/>
+      <c r="A650" s="37"/>
     </row>
     <row r="651" ht="14.25" customHeight="1">
-      <c r="A651" s="43"/>
+      <c r="A651" s="37"/>
     </row>
     <row r="652" ht="14.25" customHeight="1">
-      <c r="A652" s="43"/>
+      <c r="A652" s="37"/>
     </row>
     <row r="653" ht="14.25" customHeight="1">
-      <c r="A653" s="43"/>
+      <c r="A653" s="37"/>
     </row>
     <row r="654" ht="14.25" customHeight="1">
-      <c r="A654" s="43"/>
+      <c r="A654" s="37"/>
     </row>
     <row r="655" ht="14.25" customHeight="1">
-      <c r="A655" s="43"/>
+      <c r="A655" s="37"/>
     </row>
     <row r="656" ht="14.25" customHeight="1">
-      <c r="A656" s="43"/>
+      <c r="A656" s="37"/>
     </row>
     <row r="657" ht="14.25" customHeight="1">
-      <c r="A657" s="43"/>
+      <c r="A657" s="37"/>
     </row>
     <row r="658" ht="14.25" customHeight="1">
-      <c r="A658" s="43"/>
+      <c r="A658" s="37"/>
     </row>
     <row r="659" ht="14.25" customHeight="1">
-      <c r="A659" s="43"/>
+      <c r="A659" s="37"/>
     </row>
     <row r="660" ht="14.25" customHeight="1">
-      <c r="A660" s="43"/>
+      <c r="A660" s="37"/>
     </row>
     <row r="661" ht="14.25" customHeight="1">
-      <c r="A661" s="43"/>
+      <c r="A661" s="37"/>
     </row>
     <row r="662" ht="14.25" customHeight="1">
-      <c r="A662" s="43"/>
+      <c r="A662" s="37"/>
     </row>
     <row r="663" ht="14.25" customHeight="1">
-      <c r="A663" s="43"/>
+      <c r="A663" s="37"/>
     </row>
     <row r="664" ht="14.25" customHeight="1">
-      <c r="A664" s="43"/>
+      <c r="A664" s="37"/>
     </row>
     <row r="665" ht="14.25" customHeight="1">
-      <c r="A665" s="43"/>
+      <c r="A665" s="37"/>
     </row>
     <row r="666" ht="14.25" customHeight="1">
-      <c r="A666" s="43"/>
+      <c r="A666" s="37"/>
     </row>
     <row r="667" ht="14.25" customHeight="1">
-      <c r="A667" s="43"/>
+      <c r="A667" s="37"/>
     </row>
     <row r="668" ht="14.25" customHeight="1">
-      <c r="A668" s="43"/>
+      <c r="A668" s="37"/>
     </row>
     <row r="669" ht="14.25" customHeight="1">
-      <c r="A669" s="43"/>
+      <c r="A669" s="37"/>
     </row>
     <row r="670" ht="14.25" customHeight="1">
-      <c r="A670" s="43"/>
+      <c r="A670" s="37"/>
     </row>
     <row r="671" ht="14.25" customHeight="1">
-      <c r="A671" s="43"/>
+      <c r="A671" s="37"/>
     </row>
     <row r="672" ht="14.25" customHeight="1">
-      <c r="A672" s="43"/>
+      <c r="A672" s="37"/>
     </row>
     <row r="673" ht="14.25" customHeight="1">
-      <c r="A673" s="43"/>
+      <c r="A673" s="37"/>
     </row>
     <row r="674" ht="14.25" customHeight="1">
-      <c r="A674" s="43"/>
+      <c r="A674" s="37"/>
     </row>
     <row r="675" ht="14.25" customHeight="1">
-      <c r="A675" s="43"/>
+      <c r="A675" s="37"/>
     </row>
     <row r="676" ht="14.25" customHeight="1">
-      <c r="A676" s="43"/>
+      <c r="A676" s="37"/>
     </row>
     <row r="677" ht="14.25" customHeight="1">
-      <c r="A677" s="43"/>
+      <c r="A677" s="37"/>
     </row>
     <row r="678" ht="14.25" customHeight="1">
-      <c r="A678" s="43"/>
+      <c r="A678" s="37"/>
     </row>
     <row r="679" ht="14.25" customHeight="1">
-      <c r="A679" s="43"/>
+      <c r="A679" s="37"/>
     </row>
     <row r="680" ht="14.25" customHeight="1">
-      <c r="A680" s="43"/>
+      <c r="A680" s="37"/>
     </row>
     <row r="681" ht="14.25" customHeight="1">
-      <c r="A681" s="43"/>
+      <c r="A681" s="37"/>
     </row>
     <row r="682" ht="14.25" customHeight="1">
-      <c r="A682" s="43"/>
+      <c r="A682" s="37"/>
     </row>
     <row r="683" ht="14.25" customHeight="1">
-      <c r="A683" s="43"/>
+      <c r="A683" s="37"/>
     </row>
     <row r="684" ht="14.25" customHeight="1">
-      <c r="A684" s="43"/>
+      <c r="A684" s="37"/>
     </row>
     <row r="685" ht="14.25" customHeight="1">
-      <c r="A685" s="43"/>
+      <c r="A685" s="37"/>
     </row>
     <row r="686" ht="14.25" customHeight="1">
-      <c r="A686" s="43"/>
+      <c r="A686" s="37"/>
     </row>
     <row r="687" ht="14.25" customHeight="1">
-      <c r="A687" s="43"/>
+      <c r="A687" s="37"/>
     </row>
     <row r="688" ht="14.25" customHeight="1">
-      <c r="A688" s="43"/>
+      <c r="A688" s="37"/>
     </row>
     <row r="689" ht="14.25" customHeight="1">
-      <c r="A689" s="43"/>
+      <c r="A689" s="37"/>
     </row>
     <row r="690" ht="14.25" customHeight="1">
-      <c r="A690" s="43"/>
+      <c r="A690" s="37"/>
     </row>
     <row r="691" ht="14.25" customHeight="1">
-      <c r="A691" s="43"/>
+      <c r="A691" s="37"/>
     </row>
     <row r="692" ht="14.25" customHeight="1">
-      <c r="A692" s="43"/>
+      <c r="A692" s="37"/>
     </row>
     <row r="693" ht="14.25" customHeight="1">
-      <c r="A693" s="43"/>
+      <c r="A693" s="37"/>
     </row>
     <row r="694" ht="14.25" customHeight="1">
-      <c r="A694" s="43"/>
+      <c r="A694" s="37"/>
     </row>
     <row r="695" ht="14.25" customHeight="1">
-      <c r="A695" s="43"/>
+      <c r="A695" s="37"/>
     </row>
     <row r="696" ht="14.25" customHeight="1">
-      <c r="A696" s="43"/>
+      <c r="A696" s="37"/>
     </row>
     <row r="697" ht="14.25" customHeight="1">
-      <c r="A697" s="43"/>
+      <c r="A697" s="37"/>
     </row>
     <row r="698" ht="14.25" customHeight="1">
-      <c r="A698" s="43"/>
+      <c r="A698" s="37"/>
     </row>
     <row r="699" ht="14.25" customHeight="1">
-      <c r="A699" s="43"/>
+      <c r="A699" s="37"/>
     </row>
     <row r="700" ht="14.25" customHeight="1">
-      <c r="A700" s="43"/>
+      <c r="A700" s="37"/>
     </row>
     <row r="701" ht="14.25" customHeight="1">
-      <c r="A701" s="43"/>
+      <c r="A701" s="37"/>
     </row>
     <row r="702" ht="14.25" customHeight="1">
-      <c r="A702" s="43"/>
+      <c r="A702" s="37"/>
     </row>
     <row r="703" ht="14.25" customHeight="1">
-      <c r="A703" s="43"/>
+      <c r="A703" s="37"/>
     </row>
     <row r="704" ht="14.25" customHeight="1">
-      <c r="A704" s="43"/>
+      <c r="A704" s="37"/>
     </row>
     <row r="705" ht="14.25" customHeight="1">
-      <c r="A705" s="43"/>
+      <c r="A705" s="37"/>
     </row>
     <row r="706" ht="14.25" customHeight="1">
-      <c r="A706" s="43"/>
+      <c r="A706" s="37"/>
     </row>
     <row r="707" ht="14.25" customHeight="1">
-      <c r="A707" s="43"/>
+      <c r="A707" s="37"/>
     </row>
     <row r="708" ht="14.25" customHeight="1">
-      <c r="A708" s="43"/>
+      <c r="A708" s="37"/>
     </row>
     <row r="709" ht="14.25" customHeight="1">
-      <c r="A709" s="43"/>
+      <c r="A709" s="37"/>
     </row>
     <row r="710" ht="14.25" customHeight="1">
-      <c r="A710" s="43"/>
+      <c r="A710" s="37"/>
     </row>
     <row r="711" ht="14.25" customHeight="1">
-      <c r="A711" s="43"/>
+      <c r="A711" s="37"/>
     </row>
     <row r="712" ht="14.25" customHeight="1">
-      <c r="A712" s="43"/>
+      <c r="A712" s="37"/>
     </row>
     <row r="713" ht="14.25" customHeight="1">
-      <c r="A713" s="43"/>
+      <c r="A713" s="37"/>
     </row>
     <row r="714" ht="14.25" customHeight="1">
-      <c r="A714" s="43"/>
+      <c r="A714" s="37"/>
     </row>
     <row r="715" ht="14.25" customHeight="1">
-      <c r="A715" s="43"/>
+      <c r="A715" s="37"/>
     </row>
     <row r="716" ht="14.25" customHeight="1">
-      <c r="A716" s="43"/>
+      <c r="A716" s="37"/>
     </row>
     <row r="717" ht="14.25" customHeight="1">
-      <c r="A717" s="43"/>
+      <c r="A717" s="37"/>
     </row>
     <row r="718" ht="14.25" customHeight="1">
-      <c r="A718" s="43"/>
+      <c r="A718" s="37"/>
     </row>
     <row r="719" ht="14.25" customHeight="1">
-      <c r="A719" s="43"/>
+      <c r="A719" s="37"/>
     </row>
     <row r="720" ht="14.25" customHeight="1">
-      <c r="A720" s="43"/>
+      <c r="A720" s="37"/>
     </row>
     <row r="721" ht="14.25" customHeight="1">
-      <c r="A721" s="43"/>
+      <c r="A721" s="37"/>
     </row>
     <row r="722" ht="14.25" customHeight="1">
-      <c r="A722" s="43"/>
+      <c r="A722" s="37"/>
     </row>
     <row r="723" ht="14.25" customHeight="1">
-      <c r="A723" s="43"/>
+      <c r="A723" s="37"/>
     </row>
     <row r="724" ht="14.25" customHeight="1">
-      <c r="A724" s="43"/>
+      <c r="A724" s="37"/>
     </row>
     <row r="725" ht="14.25" customHeight="1">
-      <c r="A725" s="43"/>
+      <c r="A725" s="37"/>
     </row>
     <row r="726" ht="14.25" customHeight="1">
-      <c r="A726" s="43"/>
+      <c r="A726" s="37"/>
     </row>
     <row r="727" ht="14.25" customHeight="1">
-      <c r="A727" s="43"/>
+      <c r="A727" s="37"/>
     </row>
     <row r="728" ht="14.25" customHeight="1">
-      <c r="A728" s="43"/>
+      <c r="A728" s="37"/>
     </row>
     <row r="729" ht="14.25" customHeight="1">
-      <c r="A729" s="43"/>
+      <c r="A729" s="37"/>
     </row>
     <row r="730" ht="14.25" customHeight="1">
-      <c r="A730" s="43"/>
+      <c r="A730" s="37"/>
     </row>
     <row r="731" ht="14.25" customHeight="1">
-      <c r="A731" s="43"/>
+      <c r="A731" s="37"/>
     </row>
     <row r="732" ht="14.25" customHeight="1">
-      <c r="A732" s="43"/>
+      <c r="A732" s="37"/>
     </row>
     <row r="733" ht="14.25" customHeight="1">
-      <c r="A733" s="43"/>
+      <c r="A733" s="37"/>
     </row>
     <row r="734" ht="14.25" customHeight="1">
-      <c r="A734" s="43"/>
+      <c r="A734" s="37"/>
     </row>
     <row r="735" ht="14.25" customHeight="1">
-      <c r="A735" s="43"/>
+      <c r="A735" s="37"/>
     </row>
     <row r="736" ht="14.25" customHeight="1">
-      <c r="A736" s="43"/>
+      <c r="A736" s="37"/>
     </row>
     <row r="737" ht="14.25" customHeight="1">
-      <c r="A737" s="43"/>
+      <c r="A737" s="37"/>
     </row>
     <row r="738" ht="14.25" customHeight="1">
-      <c r="A738" s="43"/>
+      <c r="A738" s="37"/>
     </row>
     <row r="739" ht="14.25" customHeight="1">
-      <c r="A739" s="43"/>
+      <c r="A739" s="37"/>
     </row>
     <row r="740" ht="14.25" customHeight="1">
-      <c r="A740" s="43"/>
+      <c r="A740" s="37"/>
     </row>
     <row r="741" ht="14.25" customHeight="1">
-      <c r="A741" s="43"/>
+      <c r="A741" s="37"/>
     </row>
     <row r="742" ht="14.25" customHeight="1">
-      <c r="A742" s="43"/>
+      <c r="A742" s="37"/>
     </row>
     <row r="743" ht="14.25" customHeight="1">
-      <c r="A743" s="43"/>
+      <c r="A743" s="37"/>
     </row>
     <row r="744" ht="14.25" customHeight="1">
-      <c r="A744" s="43"/>
+      <c r="A744" s="37"/>
     </row>
     <row r="745" ht="14.25" customHeight="1">
-      <c r="A745" s="43"/>
+      <c r="A745" s="37"/>
     </row>
     <row r="746" ht="14.25" customHeight="1">
-      <c r="A746" s="43"/>
+      <c r="A746" s="37"/>
     </row>
     <row r="747" ht="14.25" customHeight="1">
-      <c r="A747" s="43"/>
+      <c r="A747" s="37"/>
     </row>
     <row r="748" ht="14.25" customHeight="1">
-      <c r="A748" s="43"/>
+      <c r="A748" s="37"/>
     </row>
     <row r="749" ht="14.25" customHeight="1">
-      <c r="A749" s="43"/>
+      <c r="A749" s="37"/>
     </row>
     <row r="750" ht="14.25" customHeight="1">
-      <c r="A750" s="43"/>
+      <c r="A750" s="37"/>
     </row>
     <row r="751" ht="14.25" customHeight="1">
-      <c r="A751" s="43"/>
+      <c r="A751" s="37"/>
     </row>
     <row r="752" ht="14.25" customHeight="1">
-      <c r="A752" s="43"/>
+      <c r="A752" s="37"/>
     </row>
     <row r="753" ht="14.25" customHeight="1">
-      <c r="A753" s="43"/>
+      <c r="A753" s="37"/>
     </row>
     <row r="754" ht="14.25" customHeight="1">
-      <c r="A754" s="43"/>
+      <c r="A754" s="37"/>
     </row>
     <row r="755" ht="14.25" customHeight="1">
-      <c r="A755" s="43"/>
+      <c r="A755" s="37"/>
     </row>
     <row r="756" ht="14.25" customHeight="1">
-      <c r="A756" s="43"/>
+      <c r="A756" s="37"/>
     </row>
     <row r="757" ht="14.25" customHeight="1">
-      <c r="A757" s="43"/>
+      <c r="A757" s="37"/>
     </row>
     <row r="758" ht="14.25" customHeight="1">
-      <c r="A758" s="43"/>
+      <c r="A758" s="37"/>
     </row>
     <row r="759" ht="14.25" customHeight="1">
-      <c r="A759" s="43"/>
+      <c r="A759" s="37"/>
     </row>
     <row r="760" ht="14.25" customHeight="1">
-      <c r="A760" s="43"/>
+      <c r="A760" s="37"/>
     </row>
     <row r="761" ht="14.25" customHeight="1">
-      <c r="A761" s="43"/>
+      <c r="A761" s="37"/>
     </row>
     <row r="762" ht="14.25" customHeight="1">
-      <c r="A762" s="43"/>
+      <c r="A762" s="37"/>
     </row>
     <row r="763" ht="14.25" customHeight="1">
-      <c r="A763" s="43"/>
+      <c r="A763" s="37"/>
     </row>
     <row r="764" ht="14.25" customHeight="1">
-      <c r="A764" s="43"/>
+      <c r="A764" s="37"/>
     </row>
     <row r="765" ht="14.25" customHeight="1">
-      <c r="A765" s="43"/>
+      <c r="A765" s="37"/>
     </row>
     <row r="766" ht="14.25" customHeight="1">
-      <c r="A766" s="43"/>
+      <c r="A766" s="37"/>
     </row>
     <row r="767" ht="14.25" customHeight="1">
-      <c r="A767" s="43"/>
+      <c r="A767" s="37"/>
     </row>
     <row r="768" ht="14.25" customHeight="1">
-      <c r="A768" s="43"/>
+      <c r="A768" s="37"/>
     </row>
     <row r="769" ht="14.25" customHeight="1">
-      <c r="A769" s="43"/>
+      <c r="A769" s="37"/>
     </row>
     <row r="770" ht="14.25" customHeight="1">
-      <c r="A770" s="43"/>
+      <c r="A770" s="37"/>
     </row>
     <row r="771" ht="14.25" customHeight="1">
-      <c r="A771" s="43"/>
+      <c r="A771" s="37"/>
     </row>
     <row r="772" ht="14.25" customHeight="1">
-      <c r="A772" s="43"/>
+      <c r="A772" s="37"/>
     </row>
     <row r="773" ht="14.25" customHeight="1">
-      <c r="A773" s="43"/>
+      <c r="A773" s="37"/>
     </row>
     <row r="774" ht="14.25" customHeight="1">
-      <c r="A774" s="43"/>
+      <c r="A774" s="37"/>
     </row>
     <row r="775" ht="14.25" customHeight="1">
-      <c r="A775" s="43"/>
+      <c r="A775" s="37"/>
     </row>
     <row r="776" ht="14.25" customHeight="1">
-      <c r="A776" s="43"/>
+      <c r="A776" s="37"/>
     </row>
     <row r="777" ht="14.25" customHeight="1">
-      <c r="A777" s="43"/>
+      <c r="A777" s="37"/>
     </row>
     <row r="778" ht="14.25" customHeight="1">
-      <c r="A778" s="43"/>
+      <c r="A778" s="37"/>
     </row>
     <row r="779" ht="14.25" customHeight="1">
-      <c r="A779" s="43"/>
+      <c r="A779" s="37"/>
     </row>
     <row r="780" ht="14.25" customHeight="1">
-      <c r="A780" s="43"/>
+      <c r="A780" s="37"/>
     </row>
     <row r="781" ht="14.25" customHeight="1">
-      <c r="A781" s="43"/>
+      <c r="A781" s="37"/>
     </row>
     <row r="782" ht="14.25" customHeight="1">
-      <c r="A782" s="43"/>
+      <c r="A782" s="37"/>
     </row>
     <row r="783" ht="14.25" customHeight="1">
-      <c r="A783" s="43"/>
+      <c r="A783" s="37"/>
     </row>
     <row r="784" ht="14.25" customHeight="1">
-      <c r="A784" s="43"/>
+      <c r="A784" s="37"/>
     </row>
     <row r="785" ht="14.25" customHeight="1">
-      <c r="A785" s="43"/>
+      <c r="A785" s="37"/>
     </row>
     <row r="786" ht="14.25" customHeight="1">
-      <c r="A786" s="43"/>
+      <c r="A786" s="37"/>
     </row>
     <row r="787" ht="14.25" customHeight="1">
-      <c r="A787" s="43"/>
+      <c r="A787" s="37"/>
     </row>
     <row r="788" ht="14.25" customHeight="1">
-      <c r="A788" s="43"/>
+      <c r="A788" s="37"/>
     </row>
     <row r="789" ht="14.25" customHeight="1">
-      <c r="A789" s="43"/>
+      <c r="A789" s="37"/>
     </row>
     <row r="790" ht="14.25" customHeight="1">
-      <c r="A790" s="43"/>
+      <c r="A790" s="37"/>
     </row>
     <row r="791" ht="14.25" customHeight="1">
-      <c r="A791" s="43"/>
+      <c r="A791" s="37"/>
     </row>
     <row r="792" ht="14.25" customHeight="1">
-      <c r="A792" s="43"/>
+      <c r="A792" s="37"/>
     </row>
     <row r="793" ht="14.25" customHeight="1">
-      <c r="A793" s="43"/>
+      <c r="A793" s="37"/>
     </row>
     <row r="794" ht="14.25" customHeight="1">
-      <c r="A794" s="43"/>
+      <c r="A794" s="37"/>
     </row>
     <row r="795" ht="14.25" customHeight="1">
-      <c r="A795" s="43"/>
+      <c r="A795" s="37"/>
     </row>
     <row r="796" ht="14.25" customHeight="1">
-      <c r="A796" s="43"/>
+      <c r="A796" s="37"/>
     </row>
     <row r="797" ht="14.25" customHeight="1">
-      <c r="A797" s="43"/>
+      <c r="A797" s="37"/>
     </row>
     <row r="798" ht="14.25" customHeight="1">
-      <c r="A798" s="43"/>
+      <c r="A798" s="37"/>
     </row>
     <row r="799" ht="14.25" customHeight="1">
-      <c r="A799" s="43"/>
+      <c r="A799" s="37"/>
     </row>
     <row r="800" ht="14.25" customHeight="1">
-      <c r="A800" s="43"/>
+      <c r="A800" s="37"/>
     </row>
     <row r="801" ht="14.25" customHeight="1">
-      <c r="A801" s="43"/>
+      <c r="A801" s="37"/>
     </row>
     <row r="802" ht="14.25" customHeight="1">
-      <c r="A802" s="43"/>
+      <c r="A802" s="37"/>
     </row>
     <row r="803" ht="14.25" customHeight="1">
-      <c r="A803" s="43"/>
+      <c r="A803" s="37"/>
     </row>
     <row r="804" ht="14.25" customHeight="1">
-      <c r="A804" s="43"/>
+      <c r="A804" s="37"/>
     </row>
     <row r="805" ht="14.25" customHeight="1">
-      <c r="A805" s="43"/>
+      <c r="A805" s="37"/>
     </row>
     <row r="806" ht="14.25" customHeight="1">
-      <c r="A806" s="43"/>
+      <c r="A806" s="37"/>
     </row>
     <row r="807" ht="14.25" customHeight="1">
-      <c r="A807" s="43"/>
+      <c r="A807" s="37"/>
     </row>
     <row r="808" ht="14.25" customHeight="1">
-      <c r="A808" s="43"/>
+      <c r="A808" s="37"/>
     </row>
     <row r="809" ht="14.25" customHeight="1">
-      <c r="A809" s="43"/>
+      <c r="A809" s="37"/>
     </row>
     <row r="810" ht="14.25" customHeight="1">
-      <c r="A810" s="43"/>
+      <c r="A810" s="37"/>
     </row>
     <row r="811" ht="14.25" customHeight="1">
-      <c r="A811" s="43"/>
+      <c r="A811" s="37"/>
     </row>
     <row r="812" ht="14.25" customHeight="1">
-      <c r="A812" s="43"/>
+      <c r="A812" s="37"/>
     </row>
     <row r="813" ht="14.25" customHeight="1">
-      <c r="A813" s="43"/>
+      <c r="A813" s="37"/>
     </row>
     <row r="814" ht="14.25" customHeight="1">
-      <c r="A814" s="43"/>
+      <c r="A814" s="37"/>
     </row>
     <row r="815" ht="14.25" customHeight="1">
-      <c r="A815" s="43"/>
+      <c r="A815" s="37"/>
     </row>
     <row r="816" ht="14.25" customHeight="1">
-      <c r="A816" s="43"/>
+      <c r="A816" s="37"/>
     </row>
     <row r="817" ht="14.25" customHeight="1">
-      <c r="A817" s="43"/>
+      <c r="A817" s="37"/>
     </row>
     <row r="818" ht="14.25" customHeight="1">
-      <c r="A818" s="43"/>
+      <c r="A818" s="37"/>
     </row>
     <row r="819" ht="14.25" customHeight="1">
-      <c r="A819" s="43"/>
+      <c r="A819" s="37"/>
     </row>
     <row r="820" ht="14.25" customHeight="1">
-      <c r="A820" s="43"/>
+      <c r="A820" s="37"/>
     </row>
     <row r="821" ht="14.25" customHeight="1">
-      <c r="A821" s="43"/>
+      <c r="A821" s="37"/>
     </row>
     <row r="822" ht="14.25" customHeight="1">
-      <c r="A822" s="43"/>
+      <c r="A822" s="37"/>
     </row>
     <row r="823" ht="14.25" customHeight="1">
-      <c r="A823" s="43"/>
+      <c r="A823" s="37"/>
     </row>
     <row r="824" ht="14.25" customHeight="1">
-      <c r="A824" s="43"/>
+      <c r="A824" s="37"/>
     </row>
     <row r="825" ht="14.25" customHeight="1">
-      <c r="A825" s="43"/>
+      <c r="A825" s="37"/>
     </row>
     <row r="826" ht="14.25" customHeight="1">
-      <c r="A826" s="43"/>
+      <c r="A826" s="37"/>
     </row>
     <row r="827" ht="14.25" customHeight="1">
-      <c r="A827" s="43"/>
+      <c r="A827" s="37"/>
     </row>
     <row r="828" ht="14.25" customHeight="1">
-      <c r="A828" s="43"/>
+      <c r="A828" s="37"/>
     </row>
     <row r="829" ht="14.25" customHeight="1">
-      <c r="A829" s="43"/>
+      <c r="A829" s="37"/>
     </row>
     <row r="830" ht="14.25" customHeight="1">
-      <c r="A830" s="43"/>
+      <c r="A830" s="37"/>
     </row>
     <row r="831" ht="14.25" customHeight="1">
-      <c r="A831" s="43"/>
+      <c r="A831" s="37"/>
     </row>
     <row r="832" ht="14.25" customHeight="1">
-      <c r="A832" s="43"/>
+      <c r="A832" s="37"/>
     </row>
     <row r="833" ht="14.25" customHeight="1">
-      <c r="A833" s="43"/>
+      <c r="A833" s="37"/>
     </row>
     <row r="834" ht="14.25" customHeight="1">
-      <c r="A834" s="43"/>
+      <c r="A834" s="37"/>
     </row>
     <row r="835" ht="14.25" customHeight="1">
-      <c r="A835" s="43"/>
+      <c r="A835" s="37"/>
     </row>
     <row r="836" ht="14.25" customHeight="1">
-      <c r="A836" s="43"/>
+      <c r="A836" s="37"/>
     </row>
     <row r="837" ht="14.25" customHeight="1">
-      <c r="A837" s="43"/>
+      <c r="A837" s="37"/>
     </row>
     <row r="838" ht="14.25" customHeight="1">
-      <c r="A838" s="43"/>
+      <c r="A838" s="37"/>
     </row>
     <row r="839" ht="14.25" customHeight="1">
-      <c r="A839" s="43"/>
+      <c r="A839" s="37"/>
     </row>
     <row r="840" ht="14.25" customHeight="1">
-      <c r="A840" s="43"/>
+      <c r="A840" s="37"/>
     </row>
     <row r="841" ht="14.25" customHeight="1">
-      <c r="A841" s="43"/>
+      <c r="A841" s="37"/>
     </row>
     <row r="842" ht="14.25" customHeight="1">
-      <c r="A842" s="43"/>
+      <c r="A842" s="37"/>
     </row>
     <row r="843" ht="14.25" customHeight="1">
-      <c r="A843" s="43"/>
+      <c r="A843" s="37"/>
     </row>
     <row r="844" ht="14.25" customHeight="1">
-      <c r="A844" s="43"/>
+      <c r="A844" s="37"/>
     </row>
     <row r="845" ht="14.25" customHeight="1">
-      <c r="A845" s="43"/>
+      <c r="A845" s="37"/>
     </row>
     <row r="846" ht="14.25" customHeight="1">
-      <c r="A846" s="43"/>
+      <c r="A846" s="37"/>
     </row>
     <row r="847" ht="14.25" customHeight="1">
-      <c r="A847" s="43"/>
+      <c r="A847" s="37"/>
     </row>
     <row r="848" ht="14.25" customHeight="1">
-      <c r="A848" s="43"/>
+      <c r="A848" s="37"/>
     </row>
     <row r="849" ht="14.25" customHeight="1">
-      <c r="A849" s="43"/>
+      <c r="A849" s="37"/>
     </row>
     <row r="850" ht="14.25" customHeight="1">
-      <c r="A850" s="43"/>
+      <c r="A850" s="37"/>
     </row>
     <row r="851" ht="14.25" customHeight="1">
-      <c r="A851" s="43"/>
+      <c r="A851" s="37"/>
     </row>
     <row r="852" ht="14.25" customHeight="1">
-      <c r="A852" s="43"/>
+      <c r="A852" s="37"/>
     </row>
     <row r="853" ht="14.25" customHeight="1">
-      <c r="A853" s="43"/>
+      <c r="A853" s="37"/>
     </row>
     <row r="854" ht="14.25" customHeight="1">
-      <c r="A854" s="43"/>
+      <c r="A854" s="37"/>
     </row>
     <row r="855" ht="14.25" customHeight="1">
-      <c r="A855" s="43"/>
+      <c r="A855" s="37"/>
     </row>
     <row r="856" ht="14.25" customHeight="1">
-      <c r="A856" s="43"/>
+      <c r="A856" s="37"/>
     </row>
     <row r="857" ht="14.25" customHeight="1">
-      <c r="A857" s="43"/>
+      <c r="A857" s="37"/>
     </row>
     <row r="858" ht="14.25" customHeight="1">
-      <c r="A858" s="43"/>
+      <c r="A858" s="37"/>
     </row>
     <row r="859" ht="14.25" customHeight="1">
-      <c r="A859" s="43"/>
+      <c r="A859" s="37"/>
     </row>
     <row r="860" ht="14.25" customHeight="1">
-      <c r="A860" s="43"/>
+      <c r="A860" s="37"/>
     </row>
     <row r="861" ht="14.25" customHeight="1">
-      <c r="A861" s="43"/>
+      <c r="A861" s="37"/>
     </row>
     <row r="862" ht="14.25" customHeight="1">
-      <c r="A862" s="43"/>
+      <c r="A862" s="37"/>
     </row>
     <row r="863" ht="14.25" customHeight="1">
-      <c r="A863" s="43"/>
+      <c r="A863" s="37"/>
     </row>
     <row r="864" ht="14.25" customHeight="1">
-      <c r="A864" s="43"/>
+      <c r="A864" s="37"/>
     </row>
     <row r="865" ht="14.25" customHeight="1">
-      <c r="A865" s="43"/>
+      <c r="A865" s="37"/>
     </row>
     <row r="866" ht="14.25" customHeight="1">
-      <c r="A866" s="43"/>
+      <c r="A866" s="37"/>
     </row>
     <row r="867" ht="14.25" customHeight="1">
-      <c r="A867" s="43"/>
+      <c r="A867" s="37"/>
     </row>
     <row r="868" ht="14.25" customHeight="1">
-      <c r="A868" s="43"/>
+      <c r="A868" s="37"/>
     </row>
     <row r="869" ht="14.25" customHeight="1">
-      <c r="A869" s="43"/>
+      <c r="A869" s="37"/>
     </row>
     <row r="870" ht="14.25" customHeight="1">
-      <c r="A870" s="43"/>
+      <c r="A870" s="37"/>
     </row>
     <row r="871" ht="14.25" customHeight="1">
-      <c r="A871" s="43"/>
+      <c r="A871" s="37"/>
     </row>
     <row r="872" ht="14.25" customHeight="1">
-      <c r="A872" s="43"/>
+      <c r="A872" s="37"/>
     </row>
     <row r="873" ht="14.25" customHeight="1">
-      <c r="A873" s="43"/>
+      <c r="A873" s="37"/>
     </row>
     <row r="874" ht="14.25" customHeight="1">
-      <c r="A874" s="43"/>
+      <c r="A874" s="37"/>
     </row>
     <row r="875" ht="14.25" customHeight="1">
-      <c r="A875" s="43"/>
+      <c r="A875" s="37"/>
     </row>
     <row r="876" ht="14.25" customHeight="1">
-      <c r="A876" s="43"/>
+      <c r="A876" s="37"/>
     </row>
     <row r="877" ht="14.25" customHeight="1">
-      <c r="A877" s="43"/>
+      <c r="A877" s="37"/>
     </row>
     <row r="878" ht="14.25" customHeight="1">
-      <c r="A878" s="43"/>
+      <c r="A878" s="37"/>
     </row>
     <row r="879" ht="14.25" customHeight="1">
-      <c r="A879" s="43"/>
+      <c r="A879" s="37"/>
     </row>
     <row r="880" ht="14.25" customHeight="1">
-      <c r="A880" s="43"/>
+      <c r="A880" s="37"/>
     </row>
     <row r="881" ht="14.25" customHeight="1">
-      <c r="A881" s="43"/>
+      <c r="A881" s="37"/>
     </row>
     <row r="882" ht="14.25" customHeight="1">
-      <c r="A882" s="43"/>
+      <c r="A882" s="37"/>
     </row>
     <row r="883" ht="14.25" customHeight="1">
-      <c r="A883" s="43"/>
+      <c r="A883" s="37"/>
     </row>
     <row r="884" ht="14.25" customHeight="1">
-      <c r="A884" s="43"/>
+      <c r="A884" s="37"/>
     </row>
     <row r="885" ht="14.25" customHeight="1">
-      <c r="A885" s="43"/>
+      <c r="A885" s="37"/>
     </row>
     <row r="886" ht="14.25" customHeight="1">
-      <c r="A886" s="43"/>
+      <c r="A886" s="37"/>
     </row>
     <row r="887" ht="14.25" customHeight="1">
-      <c r="A887" s="43"/>
+      <c r="A887" s="37"/>
     </row>
     <row r="888" ht="14.25" customHeight="1">
-      <c r="A888" s="43"/>
+      <c r="A888" s="37"/>
     </row>
     <row r="889" ht="14.25" customHeight="1">
-      <c r="A889" s="43"/>
+      <c r="A889" s="37"/>
     </row>
     <row r="890" ht="14.25" customHeight="1">
-      <c r="A890" s="43"/>
+      <c r="A890" s="37"/>
     </row>
     <row r="891" ht="14.25" customHeight="1">
-      <c r="A891" s="43"/>
+      <c r="A891" s="37"/>
     </row>
     <row r="892" ht="14.25" customHeight="1">
-      <c r="A892" s="43"/>
+      <c r="A892" s="37"/>
     </row>
     <row r="893" ht="14.25" customHeight="1">
-      <c r="A893" s="43"/>
+      <c r="A893" s="37"/>
     </row>
     <row r="894" ht="14.25" customHeight="1">
-      <c r="A894" s="43"/>
+      <c r="A894" s="37"/>
     </row>
     <row r="895" ht="14.25" customHeight="1">
-      <c r="A895" s="43"/>
+      <c r="A895" s="37"/>
     </row>
     <row r="896" ht="14.25" customHeight="1">
-      <c r="A896" s="43"/>
+      <c r="A896" s="37"/>
     </row>
     <row r="897" ht="14.25" customHeight="1">
-      <c r="A897" s="43"/>
+      <c r="A897" s="37"/>
     </row>
     <row r="898" ht="14.25" customHeight="1">
-      <c r="A898" s="43"/>
+      <c r="A898" s="37"/>
     </row>
     <row r="899" ht="14.25" customHeight="1">
-      <c r="A899" s="43"/>
+      <c r="A899" s="37"/>
     </row>
     <row r="900" ht="14.25" customHeight="1">
-      <c r="A900" s="43"/>
+      <c r="A900" s="37"/>
     </row>
     <row r="901" ht="14.25" customHeight="1">
-      <c r="A901" s="43"/>
+      <c r="A901" s="37"/>
     </row>
     <row r="902" ht="14.25" customHeight="1">
-      <c r="A902" s="43"/>
+      <c r="A902" s="37"/>
     </row>
     <row r="903" ht="14.25" customHeight="1">
-      <c r="A903" s="43"/>
+      <c r="A903" s="37"/>
     </row>
     <row r="904" ht="14.25" customHeight="1">
-      <c r="A904" s="43"/>
+      <c r="A904" s="37"/>
     </row>
     <row r="905" ht="14.25" customHeight="1">
-      <c r="A905" s="43"/>
+      <c r="A905" s="37"/>
     </row>
     <row r="906" ht="14.25" customHeight="1">
-      <c r="A906" s="43"/>
+      <c r="A906" s="37"/>
     </row>
     <row r="907" ht="14.25" customHeight="1">
-      <c r="A907" s="43"/>
+      <c r="A907" s="37"/>
     </row>
     <row r="908" ht="14.25" customHeight="1">
-      <c r="A908" s="43"/>
+      <c r="A908" s="37"/>
     </row>
     <row r="909" ht="14.25" customHeight="1">
-      <c r="A909" s="43"/>
+      <c r="A909" s="37"/>
     </row>
     <row r="910" ht="14.25" customHeight="1">
-      <c r="A910" s="43"/>
+      <c r="A910" s="37"/>
     </row>
     <row r="911" ht="14.25" customHeight="1">
-      <c r="A911" s="43"/>
+      <c r="A911" s="37"/>
     </row>
     <row r="912" ht="14.25" customHeight="1">
-      <c r="A912" s="43"/>
+      <c r="A912" s="37"/>
     </row>
     <row r="913" ht="14.25" customHeight="1">
-      <c r="A913" s="43"/>
+      <c r="A913" s="37"/>
     </row>
     <row r="914" ht="14.25" customHeight="1">
-      <c r="A914" s="43"/>
+      <c r="A914" s="37"/>
     </row>
     <row r="915" ht="14.25" customHeight="1">
-      <c r="A915" s="43"/>
+      <c r="A915" s="37"/>
     </row>
     <row r="916" ht="14.25" customHeight="1">
-      <c r="A916" s="43"/>
+      <c r="A916" s="37"/>
     </row>
     <row r="917" ht="14.25" customHeight="1">
-      <c r="A917" s="43"/>
+      <c r="A917" s="37"/>
     </row>
     <row r="918" ht="14.25" customHeight="1">
-      <c r="A918" s="43"/>
+      <c r="A918" s="37"/>
     </row>
     <row r="919" ht="14.25" customHeight="1">
-      <c r="A919" s="43"/>
+      <c r="A919" s="37"/>
     </row>
     <row r="920" ht="14.25" customHeight="1">
-      <c r="A920" s="43"/>
+      <c r="A920" s="37"/>
     </row>
     <row r="921" ht="14.25" customHeight="1">
-      <c r="A921" s="43"/>
+      <c r="A921" s="37"/>
     </row>
     <row r="922" ht="14.25" customHeight="1">
-      <c r="A922" s="43"/>
+      <c r="A922" s="37"/>
     </row>
     <row r="923" ht="14.25" customHeight="1">
-      <c r="A923" s="43"/>
+      <c r="A923" s="37"/>
     </row>
     <row r="924" ht="14.25" customHeight="1">
-      <c r="A924" s="43"/>
+      <c r="A924" s="37"/>
     </row>
     <row r="925" ht="14.25" customHeight="1">
-      <c r="A925" s="43"/>
+      <c r="A925" s="37"/>
     </row>
     <row r="926" ht="14.25" customHeight="1">
-      <c r="A926" s="43"/>
+      <c r="A926" s="37"/>
     </row>
     <row r="927" ht="14.25" customHeight="1">
-      <c r="A927" s="43"/>
+      <c r="A927" s="37"/>
     </row>
     <row r="928" ht="14.25" customHeight="1">
-      <c r="A928" s="43"/>
+      <c r="A928" s="37"/>
     </row>
     <row r="929" ht="14.25" customHeight="1">
-      <c r="A929" s="43"/>
+      <c r="A929" s="37"/>
     </row>
     <row r="930" ht="14.25" customHeight="1">
-      <c r="A930" s="43"/>
+      <c r="A930" s="37"/>
     </row>
     <row r="931" ht="14.25" customHeight="1">
-      <c r="A931" s="43"/>
+      <c r="A931" s="37"/>
     </row>
     <row r="932" ht="14.25" customHeight="1">
-      <c r="A932" s="43"/>
+      <c r="A932" s="37"/>
     </row>
     <row r="933" ht="14.25" customHeight="1">
-      <c r="A933" s="43"/>
+      <c r="A933" s="37"/>
     </row>
     <row r="934" ht="14.25" customHeight="1">
-      <c r="A934" s="43"/>
+      <c r="A934" s="37"/>
     </row>
     <row r="935" ht="14.25" customHeight="1">
-      <c r="A935" s="43"/>
+      <c r="A935" s="37"/>
     </row>
     <row r="936" ht="14.25" customHeight="1">
-      <c r="A936" s="43"/>
+      <c r="A936" s="37"/>
     </row>
     <row r="937" ht="14.25" customHeight="1">
-      <c r="A937" s="43"/>
+      <c r="A937" s="37"/>
     </row>
     <row r="938" ht="14.25" customHeight="1">
-      <c r="A938" s="43"/>
+      <c r="A938" s="37"/>
     </row>
     <row r="939" ht="14.25" customHeight="1">
-      <c r="A939" s="43"/>
+      <c r="A939" s="37"/>
     </row>
     <row r="940" ht="14.25" customHeight="1">
-      <c r="A940" s="43"/>
+      <c r="A940" s="37"/>
     </row>
     <row r="941" ht="14.25" customHeight="1">
-      <c r="A941" s="43"/>
+      <c r="A941" s="37"/>
     </row>
     <row r="942" ht="14.25" customHeight="1">
-      <c r="A942" s="43"/>
+      <c r="A942" s="37"/>
     </row>
     <row r="943" ht="14.25" customHeight="1">
-      <c r="A943" s="43"/>
+      <c r="A943" s="37"/>
     </row>
     <row r="944" ht="14.25" customHeight="1">
-      <c r="A944" s="43"/>
+      <c r="A944" s="37"/>
     </row>
     <row r="945" ht="14.25" customHeight="1">
-      <c r="A945" s="43"/>
+      <c r="A945" s="37"/>
     </row>
     <row r="946" ht="14.25" customHeight="1">
-      <c r="A946" s="43"/>
+      <c r="A946" s="37"/>
     </row>
     <row r="947" ht="14.25" customHeight="1">
-      <c r="A947" s="43"/>
+      <c r="A947" s="37"/>
     </row>
     <row r="948" ht="14.25" customHeight="1">
-      <c r="A948" s="43"/>
+      <c r="A948" s="37"/>
     </row>
     <row r="949" ht="14.25" customHeight="1">
-      <c r="A949" s="43"/>
+      <c r="A949" s="37"/>
     </row>
     <row r="950" ht="14.25" customHeight="1">
-      <c r="A950" s="43"/>
+      <c r="A950" s="37"/>
     </row>
     <row r="951" ht="14.25" customHeight="1">
-      <c r="A951" s="43"/>
+      <c r="A951" s="37"/>
     </row>
     <row r="952" ht="14.25" customHeight="1">
-      <c r="A952" s="43"/>
+      <c r="A952" s="37"/>
     </row>
     <row r="953" ht="14.25" customHeight="1">
-      <c r="A953" s="43"/>
+      <c r="A953" s="37"/>
     </row>
     <row r="954" ht="14.25" customHeight="1">
-      <c r="A954" s="43"/>
+      <c r="A954" s="37"/>
     </row>
     <row r="955" ht="14.25" customHeight="1">
-      <c r="A955" s="43"/>
+      <c r="A955" s="37"/>
     </row>
     <row r="956" ht="14.25" customHeight="1">
-      <c r="A956" s="43"/>
+      <c r="A956" s="37"/>
     </row>
     <row r="957" ht="14.25" customHeight="1">
-      <c r="A957" s="43"/>
+      <c r="A957" s="37"/>
     </row>
     <row r="958" ht="14.25" customHeight="1">
-      <c r="A958" s="43"/>
+      <c r="A958" s="37"/>
     </row>
     <row r="959" ht="14.25" customHeight="1">
-      <c r="A959" s="43"/>
+      <c r="A959" s="37"/>
     </row>
     <row r="960" ht="14.25" customHeight="1">
-      <c r="A960" s="43"/>
+      <c r="A960" s="37"/>
     </row>
     <row r="961" ht="14.25" customHeight="1">
-      <c r="A961" s="43"/>
+      <c r="A961" s="37"/>
     </row>
     <row r="962" ht="14.25" customHeight="1">
-      <c r="A962" s="43"/>
+      <c r="A962" s="37"/>
     </row>
     <row r="963" ht="14.25" customHeight="1">
-      <c r="A963" s="43"/>
+      <c r="A963" s="37"/>
     </row>
     <row r="964" ht="14.25" customHeight="1">
-      <c r="A964" s="43"/>
+      <c r="A964" s="37"/>
     </row>
     <row r="965" ht="14.25" customHeight="1">
-      <c r="A965" s="43"/>
+      <c r="A965" s="37"/>
     </row>
     <row r="966" ht="14.25" customHeight="1">
-      <c r="A966" s="43"/>
+      <c r="A966" s="37"/>
     </row>
     <row r="967" ht="14.25" customHeight="1">
-      <c r="A967" s="43"/>
+      <c r="A967" s="37"/>
     </row>
     <row r="968" ht="14.25" customHeight="1">
-      <c r="A968" s="43"/>
+      <c r="A968" s="37"/>
     </row>
     <row r="969" ht="14.25" customHeight="1">
-      <c r="A969" s="43"/>
+      <c r="A969" s="37"/>
     </row>
     <row r="970" ht="14.25" customHeight="1">
-      <c r="A970" s="43"/>
+      <c r="A970" s="37"/>
     </row>
     <row r="971" ht="14.25" customHeight="1">
-      <c r="A971" s="43"/>
+      <c r="A971" s="37"/>
     </row>
     <row r="972" ht="14.25" customHeight="1">
-      <c r="A972" s="43"/>
+      <c r="A972" s="37"/>
     </row>
     <row r="973" ht="14.25" customHeight="1">
-      <c r="A973" s="43"/>
+      <c r="A973" s="37"/>
     </row>
     <row r="974" ht="14.25" customHeight="1">
-      <c r="A974" s="43"/>
+      <c r="A974" s="37"/>
     </row>
     <row r="975" ht="14.25" customHeight="1">
-      <c r="A975" s="43"/>
+      <c r="A975" s="37"/>
     </row>
     <row r="976" ht="14.25" customHeight="1">
-      <c r="A976" s="43"/>
+      <c r="A976" s="37"/>
     </row>
     <row r="977" ht="14.25" customHeight="1">
-      <c r="A977" s="43"/>
+      <c r="A977" s="37"/>
     </row>
     <row r="978" ht="14.25" customHeight="1">
-      <c r="A978" s="43"/>
+      <c r="A978" s="37"/>
     </row>
     <row r="979" ht="14.25" customHeight="1">
-      <c r="A979" s="43"/>
+      <c r="A979" s="37"/>
     </row>
     <row r="980" ht="14.25" customHeight="1">
-      <c r="A980" s="43"/>
+      <c r="A980" s="37"/>
     </row>
     <row r="981" ht="14.25" customHeight="1">
-      <c r="A981" s="43"/>
+      <c r="A981" s="37"/>
     </row>
     <row r="982" ht="14.25" customHeight="1">
-      <c r="A982" s="43"/>
+      <c r="A982" s="37"/>
     </row>
     <row r="983" ht="14.25" customHeight="1">
-      <c r="A983" s="43"/>
+      <c r="A983" s="37"/>
     </row>
     <row r="984" ht="14.25" customHeight="1">
-      <c r="A984" s="43"/>
+      <c r="A984" s="37"/>
     </row>
     <row r="985" ht="14.25" customHeight="1">
-      <c r="A985" s="43"/>
+      <c r="A985" s="37"/>
     </row>
     <row r="986" ht="14.25" customHeight="1">
-      <c r="A986" s="43"/>
+      <c r="A986" s="37"/>
     </row>
     <row r="987" ht="14.25" customHeight="1">
-      <c r="A987" s="43"/>
+      <c r="A987" s="37"/>
     </row>
     <row r="988" ht="14.25" customHeight="1">
-      <c r="A988" s="43"/>
+      <c r="A988" s="37"/>
     </row>
     <row r="989" ht="14.25" customHeight="1">
-      <c r="A989" s="43"/>
+      <c r="A989" s="37"/>
     </row>
     <row r="990" ht="14.25" customHeight="1">
-      <c r="A990" s="43"/>
+      <c r="A990" s="37"/>
     </row>
     <row r="991" ht="14.25" customHeight="1">
-      <c r="A991" s="43"/>
+      <c r="A991" s="37"/>
     </row>
     <row r="992" ht="14.25" customHeight="1">
-      <c r="A992" s="43"/>
+      <c r="A992" s="37"/>
     </row>
     <row r="993" ht="14.25" customHeight="1">
-      <c r="A993" s="43"/>
+      <c r="A993" s="37"/>
     </row>
     <row r="994" ht="14.25" customHeight="1">
-      <c r="A994" s="43"/>
+      <c r="A994" s="37"/>
     </row>
     <row r="995" ht="14.25" customHeight="1">
-      <c r="A995" s="43"/>
+      <c r="A995" s="37"/>
     </row>
     <row r="996" ht="14.25" customHeight="1">
-      <c r="A996" s="43"/>
+      <c r="A996" s="37"/>
     </row>
     <row r="997" ht="14.25" customHeight="1">
-      <c r="A997" s="43"/>
+      <c r="A997" s="37"/>
     </row>
     <row r="998" ht="14.25" customHeight="1">
-      <c r="A998" s="43"/>
+      <c r="A998" s="37"/>
     </row>
     <row r="999" ht="14.25" customHeight="1">
-      <c r="A999" s="43"/>
+      <c r="A999" s="37"/>
     </row>
     <row r="1000" ht="14.25" customHeight="1">
-      <c r="A1000" s="43"/>
+      <c r="A1000" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>